<commit_message>
Update Laser.xlsx from Google Sheets @ 2025-10-27T14:18:44.951Z
</commit_message>
<xml_diff>
--- a/Laser.xlsx
+++ b/Laser.xlsx
@@ -254,10 +254,10 @@
     <xf borderId="4" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="5" fillId="2" fontId="3" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="5" fillId="2" fontId="3" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -690,11 +690,13 @@
         <v>10.0</v>
       </c>
       <c r="D7" s="11">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
-      <c r="E7" s="12"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
+      <c r="E7" s="14">
+        <v>45957.92965825232</v>
+      </c>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
@@ -716,11 +718,11 @@
       <c r="D8" s="11">
         <v>1.0</v>
       </c>
-      <c r="E8" s="15">
+      <c r="E8" s="14">
         <v>45954.915123425926</v>
       </c>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
@@ -17049,9 +17051,9 @@
         <v>1.0</v>
       </c>
       <c r="E6" s="23"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
@@ -17074,9 +17076,9 @@
         <v>1.0</v>
       </c>
       <c r="E7" s="24"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>

</xml_diff>

<commit_message>
Update Laser.xlsx from Google Sheets @ 2025-10-30T15:27:33.197Z
</commit_message>
<xml_diff>
--- a/Laser.xlsx
+++ b/Laser.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="24">
   <si>
     <t>項目</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>(PS)</t>
+  </si>
+  <si>
+    <t>Fill</t>
   </si>
   <si>
     <t>遮蓋膠紙</t>
@@ -17178,11 +17181,21 @@
       <c r="O11" s="4"/>
     </row>
     <row r="12">
-      <c r="A12" s="13"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="26"/>
+      <c r="A12" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="11">
+        <v>4.0</v>
+      </c>
+      <c r="C12" s="11">
+        <v>10.0</v>
+      </c>
+      <c r="D12" s="11">
+        <v>1.0</v>
+      </c>
+      <c r="E12" s="25">
+        <v>45960.97744890046</v>
+      </c>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
@@ -34371,10 +34384,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
@@ -34451,7 +34464,7 @@
     </row>
     <row r="5">
       <c r="A5" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
@@ -34493,7 +34506,7 @@
     </row>
     <row r="7">
       <c r="A7" s="7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B7" s="8">
         <v>20.0</v>
@@ -34689,7 +34702,7 @@
     </row>
     <row r="17">
       <c r="A17" s="34" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B17" s="17"/>
       <c r="C17" s="17"/>
@@ -34706,7 +34719,7 @@
     </row>
     <row r="18">
       <c r="A18" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B18" s="30">
         <v>2.0</v>
@@ -34796,10 +34809,10 @@
     </row>
     <row r="22">
       <c r="A22" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>

</xml_diff>

<commit_message>
Update Laser.xlsx from Google Sheets @ 2025-11-13T13:13:28.744Z
</commit_message>
<xml_diff>
--- a/Laser.xlsx
+++ b/Laser.xlsx
@@ -17519,9 +17519,11 @@
         <v>5.0</v>
       </c>
       <c r="D27" s="8">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
-      <c r="E27" s="23"/>
+      <c r="E27" s="24">
+        <v>45974.8842990625</v>
+      </c>
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>

</xml_diff>

<commit_message>
Update Laser.xlsx from Google Sheets @ 2025-12-15T14:33:34.901Z
</commit_message>
<xml_diff>
--- a/Laser.xlsx
+++ b/Laser.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="25">
   <si>
     <t>項目</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>Cut</t>
+  </si>
+  <si>
+    <t>６</t>
   </si>
   <si>
     <t>5mm</t>
@@ -34645,8 +34648,8 @@
       <c r="A14" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="33">
-        <v>5.0</v>
+      <c r="B14" s="33" t="s">
+        <v>20</v>
       </c>
       <c r="C14" s="33">
         <v>20.0</v>
@@ -34654,7 +34657,9 @@
       <c r="D14" s="33">
         <v>1.0</v>
       </c>
-      <c r="E14" s="26"/>
+      <c r="E14" s="25">
+        <v>46006.93993954861</v>
+      </c>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
@@ -34704,7 +34709,7 @@
     </row>
     <row r="17">
       <c r="A17" s="34" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B17" s="17"/>
       <c r="C17" s="17"/>
@@ -34721,7 +34726,7 @@
     </row>
     <row r="18">
       <c r="A18" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B18" s="30">
         <v>2.0</v>
@@ -34811,10 +34816,10 @@
     </row>
     <row r="22">
       <c r="A22" s="7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>

</xml_diff>

<commit_message>
Update Laser.xlsx from Google Sheets @ 2025-12-15T14:56:05.381Z
</commit_message>
<xml_diff>
--- a/Laser.xlsx
+++ b/Laser.xlsx
@@ -34708,9 +34708,7 @@
       <c r="M16" s="4"/>
     </row>
     <row r="17">
-      <c r="A17" s="34" t="s">
-        <v>21</v>
-      </c>
+      <c r="A17" s="16"/>
       <c r="B17" s="17"/>
       <c r="C17" s="17"/>
       <c r="D17" s="17"/>
@@ -34725,21 +34723,11 @@
       <c r="M17" s="4"/>
     </row>
     <row r="18">
-      <c r="A18" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18" s="30">
-        <v>2.0</v>
-      </c>
-      <c r="C18" s="30">
-        <v>100.0</v>
-      </c>
-      <c r="D18" s="30">
-        <v>1.0</v>
-      </c>
-      <c r="E18" s="24">
-        <v>45900.48749</v>
-      </c>
+      <c r="A18" s="16"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="23"/>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
@@ -34750,21 +34738,13 @@
       <c r="M18" s="4"/>
     </row>
     <row r="19">
-      <c r="A19" s="7" t="s">
-        <v>6</v>
+      <c r="A19" s="34" t="s">
+        <v>21</v>
       </c>
-      <c r="B19" s="30">
-        <v>2.0</v>
-      </c>
-      <c r="C19" s="30">
-        <v>85.0</v>
-      </c>
-      <c r="D19" s="30">
-        <v>1.0</v>
-      </c>
-      <c r="E19" s="24">
-        <v>45900.48745738426</v>
-      </c>
+      <c r="B19" s="17"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="23"/>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
@@ -34776,19 +34756,19 @@
     </row>
     <row r="20">
       <c r="A20" s="7" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="B20" s="30">
-        <v>70.0</v>
+        <v>2.0</v>
       </c>
       <c r="C20" s="30">
-        <v>10.0</v>
+        <v>100.0</v>
       </c>
       <c r="D20" s="30">
         <v>1.0</v>
       </c>
       <c r="E20" s="24">
-        <v>45900.48752491898</v>
+        <v>45900.48749</v>
       </c>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
@@ -34800,11 +34780,21 @@
       <c r="M20" s="4"/>
     </row>
     <row r="21">
-      <c r="A21" s="7"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="23"/>
+      <c r="A21" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="30">
+        <v>2.0</v>
+      </c>
+      <c r="C21" s="30">
+        <v>85.0</v>
+      </c>
+      <c r="D21" s="30">
+        <v>1.0</v>
+      </c>
+      <c r="E21" s="24">
+        <v>45900.48745738426</v>
+      </c>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
@@ -34816,15 +34806,19 @@
     </row>
     <row r="22">
       <c r="A22" s="7" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
-      <c r="B22" s="8" t="s">
-        <v>24</v>
+      <c r="B22" s="30">
+        <v>70.0</v>
       </c>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
+      <c r="C22" s="30">
+        <v>10.0</v>
+      </c>
+      <c r="D22" s="30">
+        <v>1.0</v>
+      </c>
       <c r="E22" s="24">
-        <v>45946.87875708334</v>
+        <v>45900.48752491898</v>
       </c>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
@@ -34836,17 +34830,11 @@
       <c r="M22" s="4"/>
     </row>
     <row r="23">
-      <c r="A23" s="7">
-        <v>50.0</v>
-      </c>
-      <c r="B23" s="8">
-        <v>100.0</v>
-      </c>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="24">
-        <v>45946.87887299768</v>
-      </c>
+      <c r="A23" s="7"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="23"/>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
@@ -34857,11 +34845,17 @@
       <c r="M23" s="4"/>
     </row>
     <row r="24">
-      <c r="A24" s="35"/>
-      <c r="B24" s="36"/>
-      <c r="C24" s="36"/>
-      <c r="D24" s="36"/>
-      <c r="E24" s="37"/>
+      <c r="A24" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="24">
+        <v>45946.87875708334</v>
+      </c>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
@@ -34872,11 +34866,17 @@
       <c r="M24" s="4"/>
     </row>
     <row r="25">
-      <c r="A25" s="38"/>
-      <c r="B25" s="38"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
+      <c r="A25" s="7">
+        <v>50.0</v>
+      </c>
+      <c r="B25" s="8">
+        <v>100.0</v>
+      </c>
+      <c r="C25" s="17"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="24">
+        <v>45946.87887299768</v>
+      </c>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
@@ -34887,11 +34887,11 @@
       <c r="M25" s="4"/>
     </row>
     <row r="26">
-      <c r="A26" s="38"/>
-      <c r="B26" s="38"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
+      <c r="A26" s="35"/>
+      <c r="B26" s="36"/>
+      <c r="C26" s="36"/>
+      <c r="D26" s="36"/>
+      <c r="E26" s="37"/>
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
@@ -35142,8 +35142,8 @@
       <c r="M42" s="4"/>
     </row>
     <row r="43">
-      <c r="A43" s="4"/>
-      <c r="B43" s="4"/>
+      <c r="A43" s="38"/>
+      <c r="B43" s="38"/>
       <c r="C43" s="4"/>
       <c r="D43" s="4"/>
       <c r="E43" s="4"/>
@@ -35157,8 +35157,8 @@
       <c r="M43" s="4"/>
     </row>
     <row r="44">
-      <c r="A44" s="4"/>
-      <c r="B44" s="4"/>
+      <c r="A44" s="38"/>
+      <c r="B44" s="38"/>
       <c r="C44" s="4"/>
       <c r="D44" s="4"/>
       <c r="E44" s="4"/>
@@ -49211,6 +49211,36 @@
       <c r="L980" s="4"/>
       <c r="M980" s="4"/>
     </row>
+    <row r="981">
+      <c r="A981" s="4"/>
+      <c r="B981" s="4"/>
+      <c r="C981" s="4"/>
+      <c r="D981" s="4"/>
+      <c r="E981" s="4"/>
+      <c r="F981" s="4"/>
+      <c r="G981" s="4"/>
+      <c r="H981" s="4"/>
+      <c r="I981" s="4"/>
+      <c r="J981" s="4"/>
+      <c r="K981" s="4"/>
+      <c r="L981" s="4"/>
+      <c r="M981" s="4"/>
+    </row>
+    <row r="982">
+      <c r="A982" s="4"/>
+      <c r="B982" s="4"/>
+      <c r="C982" s="4"/>
+      <c r="D982" s="4"/>
+      <c r="E982" s="4"/>
+      <c r="F982" s="4"/>
+      <c r="G982" s="4"/>
+      <c r="H982" s="4"/>
+      <c r="I982" s="4"/>
+      <c r="J982" s="4"/>
+      <c r="K982" s="4"/>
+      <c r="L982" s="4"/>
+      <c r="M982" s="4"/>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Laser.xlsx from Google Sheets @ 2025-12-15T14:56:07.724Z
</commit_message>
<xml_diff>
--- a/Laser.xlsx
+++ b/Laser.xlsx
@@ -34738,9 +34738,7 @@
       <c r="M18" s="4"/>
     </row>
     <row r="19">
-      <c r="A19" s="34" t="s">
-        <v>21</v>
-      </c>
+      <c r="A19" s="16"/>
       <c r="B19" s="17"/>
       <c r="C19" s="17"/>
       <c r="D19" s="17"/>
@@ -34755,21 +34753,13 @@
       <c r="M19" s="4"/>
     </row>
     <row r="20">
-      <c r="A20" s="7" t="s">
-        <v>22</v>
+      <c r="A20" s="34" t="s">
+        <v>21</v>
       </c>
-      <c r="B20" s="30">
-        <v>2.0</v>
-      </c>
-      <c r="C20" s="30">
-        <v>100.0</v>
-      </c>
-      <c r="D20" s="30">
-        <v>1.0</v>
-      </c>
-      <c r="E20" s="24">
-        <v>45900.48749</v>
-      </c>
+      <c r="B20" s="17"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="23"/>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
@@ -34781,19 +34771,19 @@
     </row>
     <row r="21">
       <c r="A21" s="7" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="B21" s="30">
         <v>2.0</v>
       </c>
       <c r="C21" s="30">
-        <v>85.0</v>
+        <v>100.0</v>
       </c>
       <c r="D21" s="30">
         <v>1.0</v>
       </c>
       <c r="E21" s="24">
-        <v>45900.48745738426</v>
+        <v>45900.48749</v>
       </c>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
@@ -34806,19 +34796,19 @@
     </row>
     <row r="22">
       <c r="A22" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B22" s="30">
-        <v>70.0</v>
+        <v>2.0</v>
       </c>
       <c r="C22" s="30">
-        <v>10.0</v>
+        <v>85.0</v>
       </c>
       <c r="D22" s="30">
         <v>1.0</v>
       </c>
       <c r="E22" s="24">
-        <v>45900.48752491898</v>
+        <v>45900.48745738426</v>
       </c>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
@@ -34830,11 +34820,21 @@
       <c r="M22" s="4"/>
     </row>
     <row r="23">
-      <c r="A23" s="7"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="23"/>
+      <c r="A23" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" s="30">
+        <v>70.0</v>
+      </c>
+      <c r="C23" s="30">
+        <v>10.0</v>
+      </c>
+      <c r="D23" s="30">
+        <v>1.0</v>
+      </c>
+      <c r="E23" s="24">
+        <v>45900.48752491898</v>
+      </c>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
@@ -34845,17 +34845,11 @@
       <c r="M23" s="4"/>
     </row>
     <row r="24">
-      <c r="A24" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>24</v>
-      </c>
+      <c r="A24" s="7"/>
+      <c r="B24" s="8"/>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
-      <c r="E24" s="24">
-        <v>45946.87875708334</v>
-      </c>
+      <c r="E24" s="23"/>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
@@ -34866,16 +34860,16 @@
       <c r="M24" s="4"/>
     </row>
     <row r="25">
-      <c r="A25" s="7">
-        <v>50.0</v>
+      <c r="A25" s="7" t="s">
+        <v>23</v>
       </c>
-      <c r="B25" s="8">
-        <v>100.0</v>
+      <c r="B25" s="8" t="s">
+        <v>24</v>
       </c>
-      <c r="C25" s="17"/>
-      <c r="D25" s="17"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
       <c r="E25" s="24">
-        <v>45946.87887299768</v>
+        <v>45946.87875708334</v>
       </c>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
@@ -34887,11 +34881,17 @@
       <c r="M25" s="4"/>
     </row>
     <row r="26">
-      <c r="A26" s="35"/>
-      <c r="B26" s="36"/>
-      <c r="C26" s="36"/>
-      <c r="D26" s="36"/>
-      <c r="E26" s="37"/>
+      <c r="A26" s="7">
+        <v>50.0</v>
+      </c>
+      <c r="B26" s="8">
+        <v>100.0</v>
+      </c>
+      <c r="C26" s="17"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="24">
+        <v>45946.87887299768</v>
+      </c>
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
@@ -34902,11 +34902,11 @@
       <c r="M26" s="4"/>
     </row>
     <row r="27">
-      <c r="A27" s="38"/>
-      <c r="B27" s="38"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
+      <c r="A27" s="35"/>
+      <c r="B27" s="36"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="36"/>
+      <c r="E27" s="37"/>
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
@@ -35172,8 +35172,8 @@
       <c r="M44" s="4"/>
     </row>
     <row r="45">
-      <c r="A45" s="4"/>
-      <c r="B45" s="4"/>
+      <c r="A45" s="38"/>
+      <c r="B45" s="38"/>
       <c r="C45" s="4"/>
       <c r="D45" s="4"/>
       <c r="E45" s="4"/>
@@ -49241,6 +49241,21 @@
       <c r="L982" s="4"/>
       <c r="M982" s="4"/>
     </row>
+    <row r="983">
+      <c r="A983" s="4"/>
+      <c r="B983" s="4"/>
+      <c r="C983" s="4"/>
+      <c r="D983" s="4"/>
+      <c r="E983" s="4"/>
+      <c r="F983" s="4"/>
+      <c r="G983" s="4"/>
+      <c r="H983" s="4"/>
+      <c r="I983" s="4"/>
+      <c r="J983" s="4"/>
+      <c r="K983" s="4"/>
+      <c r="L983" s="4"/>
+      <c r="M983" s="4"/>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Laser.xlsx from Google Sheets @ 2025-12-15T14:56:14.790Z
</commit_message>
<xml_diff>
--- a/Laser.xlsx
+++ b/Laser.xlsx
@@ -34753,9 +34753,7 @@
       <c r="M19" s="4"/>
     </row>
     <row r="20">
-      <c r="A20" s="34" t="s">
-        <v>21</v>
-      </c>
+      <c r="A20" s="16"/>
       <c r="B20" s="17"/>
       <c r="C20" s="17"/>
       <c r="D20" s="17"/>
@@ -34770,21 +34768,13 @@
       <c r="M20" s="4"/>
     </row>
     <row r="21">
-      <c r="A21" s="7" t="s">
-        <v>22</v>
+      <c r="A21" s="34" t="s">
+        <v>21</v>
       </c>
-      <c r="B21" s="30">
-        <v>2.0</v>
-      </c>
-      <c r="C21" s="30">
-        <v>100.0</v>
-      </c>
-      <c r="D21" s="30">
-        <v>1.0</v>
-      </c>
-      <c r="E21" s="24">
-        <v>45900.48749</v>
-      </c>
+      <c r="B21" s="17"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="23"/>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
@@ -34796,19 +34786,19 @@
     </row>
     <row r="22">
       <c r="A22" s="7" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="B22" s="30">
         <v>2.0</v>
       </c>
       <c r="C22" s="30">
-        <v>85.0</v>
+        <v>100.0</v>
       </c>
       <c r="D22" s="30">
         <v>1.0</v>
       </c>
       <c r="E22" s="24">
-        <v>45900.48745738426</v>
+        <v>45900.48749</v>
       </c>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
@@ -34821,19 +34811,19 @@
     </row>
     <row r="23">
       <c r="A23" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B23" s="30">
-        <v>70.0</v>
+        <v>2.0</v>
       </c>
       <c r="C23" s="30">
-        <v>10.0</v>
+        <v>85.0</v>
       </c>
       <c r="D23" s="30">
         <v>1.0</v>
       </c>
       <c r="E23" s="24">
-        <v>45900.48752491898</v>
+        <v>45900.48745738426</v>
       </c>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
@@ -34845,11 +34835,21 @@
       <c r="M23" s="4"/>
     </row>
     <row r="24">
-      <c r="A24" s="7"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="23"/>
+      <c r="A24" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" s="30">
+        <v>70.0</v>
+      </c>
+      <c r="C24" s="30">
+        <v>10.0</v>
+      </c>
+      <c r="D24" s="30">
+        <v>1.0</v>
+      </c>
+      <c r="E24" s="24">
+        <v>45900.48752491898</v>
+      </c>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
@@ -34860,17 +34860,11 @@
       <c r="M24" s="4"/>
     </row>
     <row r="25">
-      <c r="A25" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>24</v>
-      </c>
+      <c r="A25" s="7"/>
+      <c r="B25" s="8"/>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
-      <c r="E25" s="24">
-        <v>45946.87875708334</v>
-      </c>
+      <c r="E25" s="23"/>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
@@ -34881,16 +34875,16 @@
       <c r="M25" s="4"/>
     </row>
     <row r="26">
-      <c r="A26" s="7">
-        <v>50.0</v>
+      <c r="A26" s="7" t="s">
+        <v>23</v>
       </c>
-      <c r="B26" s="8">
-        <v>100.0</v>
+      <c r="B26" s="8" t="s">
+        <v>24</v>
       </c>
-      <c r="C26" s="17"/>
-      <c r="D26" s="17"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
       <c r="E26" s="24">
-        <v>45946.87887299768</v>
+        <v>45946.87875708334</v>
       </c>
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
@@ -34902,11 +34896,17 @@
       <c r="M26" s="4"/>
     </row>
     <row r="27">
-      <c r="A27" s="35"/>
-      <c r="B27" s="36"/>
-      <c r="C27" s="36"/>
-      <c r="D27" s="36"/>
-      <c r="E27" s="37"/>
+      <c r="A27" s="7">
+        <v>50.0</v>
+      </c>
+      <c r="B27" s="8">
+        <v>100.0</v>
+      </c>
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="24">
+        <v>45946.87887299768</v>
+      </c>
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
@@ -34917,11 +34917,11 @@
       <c r="M27" s="4"/>
     </row>
     <row r="28">
-      <c r="A28" s="38"/>
-      <c r="B28" s="38"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
+      <c r="A28" s="35"/>
+      <c r="B28" s="36"/>
+      <c r="C28" s="36"/>
+      <c r="D28" s="36"/>
+      <c r="E28" s="37"/>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
@@ -35187,8 +35187,8 @@
       <c r="M45" s="4"/>
     </row>
     <row r="46">
-      <c r="A46" s="4"/>
-      <c r="B46" s="4"/>
+      <c r="A46" s="38"/>
+      <c r="B46" s="38"/>
       <c r="C46" s="4"/>
       <c r="D46" s="4"/>
       <c r="E46" s="4"/>
@@ -49256,6 +49256,21 @@
       <c r="L983" s="4"/>
       <c r="M983" s="4"/>
     </row>
+    <row r="984">
+      <c r="A984" s="4"/>
+      <c r="B984" s="4"/>
+      <c r="C984" s="4"/>
+      <c r="D984" s="4"/>
+      <c r="E984" s="4"/>
+      <c r="F984" s="4"/>
+      <c r="G984" s="4"/>
+      <c r="H984" s="4"/>
+      <c r="I984" s="4"/>
+      <c r="J984" s="4"/>
+      <c r="K984" s="4"/>
+      <c r="L984" s="4"/>
+      <c r="M984" s="4"/>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Laser.xlsx from Google Sheets @ 2025-12-15T14:56:29.547Z
</commit_message>
<xml_diff>
--- a/Laser.xlsx
+++ b/Laser.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="25">
   <si>
     <t>項目</t>
   </si>
@@ -34708,7 +34708,9 @@
       <c r="M16" s="4"/>
     </row>
     <row r="17">
-      <c r="A17" s="16"/>
+      <c r="A17" s="7" t="s">
+        <v>10</v>
+      </c>
       <c r="B17" s="17"/>
       <c r="C17" s="17"/>
       <c r="D17" s="17"/>

</xml_diff>

<commit_message>
Update Laser.xlsx from Google Sheets @ 2025-12-15T14:56:35.051Z
</commit_message>
<xml_diff>
--- a/Laser.xlsx
+++ b/Laser.xlsx
@@ -34708,8 +34708,8 @@
       <c r="M16" s="4"/>
     </row>
     <row r="17">
-      <c r="A17" s="7" t="s">
-        <v>10</v>
+      <c r="A17" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="B17" s="17"/>
       <c r="C17" s="17"/>

</xml_diff>

<commit_message>
Update Laser.xlsx from Google Sheets @ 2025-12-15T14:56:39.217Z
</commit_message>
<xml_diff>
--- a/Laser.xlsx
+++ b/Laser.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="25">
   <si>
     <t>項目</t>
   </si>
@@ -34725,7 +34725,9 @@
       <c r="M17" s="4"/>
     </row>
     <row r="18">
-      <c r="A18" s="16"/>
+      <c r="A18" s="7" t="s">
+        <v>6</v>
+      </c>
       <c r="B18" s="17"/>
       <c r="C18" s="17"/>
       <c r="D18" s="17"/>

</xml_diff>

<commit_message>
Update Laser.xlsx from Google Sheets @ 2025-12-15T14:56:43.018Z
</commit_message>
<xml_diff>
--- a/Laser.xlsx
+++ b/Laser.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="25">
   <si>
     <t>項目</t>
   </si>
@@ -34742,7 +34742,9 @@
       <c r="M18" s="4"/>
     </row>
     <row r="19">
-      <c r="A19" s="16"/>
+      <c r="A19" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="B19" s="17"/>
       <c r="C19" s="17"/>
       <c r="D19" s="17"/>

</xml_diff>

<commit_message>
Update Laser.xlsx from Google Sheets @ 2025-12-15T14:56:47.643Z
</commit_message>
<xml_diff>
--- a/Laser.xlsx
+++ b/Laser.xlsx
@@ -34728,10 +34728,14 @@
       <c r="A18" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="17"/>
+      <c r="B18" s="8">
+        <v>9.0</v>
+      </c>
       <c r="C18" s="17"/>
       <c r="D18" s="17"/>
-      <c r="E18" s="23"/>
+      <c r="E18" s="24">
+        <v>46006.95608604167</v>
+      </c>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>

</xml_diff>

<commit_message>
Update Laser.xlsx from Google Sheets @ 2025-12-15T14:56:54.760Z
</commit_message>
<xml_diff>
--- a/Laser.xlsx
+++ b/Laser.xlsx
@@ -34731,10 +34731,12 @@
       <c r="B18" s="8">
         <v>9.0</v>
       </c>
-      <c r="C18" s="17"/>
+      <c r="C18" s="8">
+        <v>20.0</v>
+      </c>
       <c r="D18" s="17"/>
       <c r="E18" s="24">
-        <v>46006.95608604167</v>
+        <v>46006.95616824074</v>
       </c>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>

</xml_diff>

<commit_message>
Update Laser.xlsx from Google Sheets @ 2025-12-15T14:56:59.033Z
</commit_message>
<xml_diff>
--- a/Laser.xlsx
+++ b/Laser.xlsx
@@ -34734,9 +34734,11 @@
       <c r="C18" s="8">
         <v>20.0</v>
       </c>
-      <c r="D18" s="17"/>
+      <c r="D18" s="8">
+        <v>1.0</v>
+      </c>
       <c r="E18" s="24">
-        <v>46006.95616824074</v>
+        <v>46006.95620635417</v>
       </c>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
@@ -34753,8 +34755,12 @@
       </c>
       <c r="B19" s="17"/>
       <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="23"/>
+      <c r="D19" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="E19" s="24">
+        <v>46006.9562227662</v>
+      </c>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>

</xml_diff>

<commit_message>
Update Laser.xlsx from Google Sheets @ 2025-12-15T14:57:04.046Z
</commit_message>
<xml_diff>
--- a/Laser.xlsx
+++ b/Laser.xlsx
@@ -34753,13 +34753,17 @@
       <c r="A19" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="17"/>
-      <c r="C19" s="17"/>
+      <c r="B19" s="8">
+        <v>55.0</v>
+      </c>
+      <c r="C19" s="8">
+        <v>20.0</v>
+      </c>
       <c r="D19" s="8">
         <v>1.0</v>
       </c>
       <c r="E19" s="24">
-        <v>46006.9562227662</v>
+        <v>46006.95627618056</v>
       </c>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>

</xml_diff>

<commit_message>
Update Laser.xlsx from Google Sheets @ 2025-12-18T10:47:46.411Z
</commit_message>
<xml_diff>
--- a/Laser.xlsx
+++ b/Laser.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="26">
   <si>
     <t>項目</t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t>切割%</t>
+  </si>
+  <si>
+    <t>20mm</t>
   </si>
 </sst>
 </file>
@@ -34939,7 +34942,9 @@
       <c r="M27" s="4"/>
     </row>
     <row r="28">
-      <c r="A28" s="35"/>
+      <c r="A28" s="35" t="s">
+        <v>25</v>
+      </c>
       <c r="B28" s="36"/>
       <c r="C28" s="36"/>
       <c r="D28" s="36"/>

</xml_diff>

<commit_message>
Update Laser.xlsx from Google Sheets @ 2025-12-18T10:48:03.324Z
</commit_message>
<xml_diff>
--- a/Laser.xlsx
+++ b/Laser.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="27">
   <si>
     <t>項目</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>20mm</t>
+  </si>
+  <si>
+    <t>Cut1-2</t>
   </si>
 </sst>
 </file>
@@ -220,7 +223,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -332,6 +335,9 @@
     </xf>
     <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
@@ -34959,8 +34965,10 @@
       <c r="M28" s="4"/>
     </row>
     <row r="29">
-      <c r="A29" s="38"/>
-      <c r="B29" s="38"/>
+      <c r="A29" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29" s="39"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
@@ -34974,8 +34982,8 @@
       <c r="M29" s="4"/>
     </row>
     <row r="30">
-      <c r="A30" s="38"/>
-      <c r="B30" s="38"/>
+      <c r="A30" s="39"/>
+      <c r="B30" s="39"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
@@ -34989,8 +34997,8 @@
       <c r="M30" s="4"/>
     </row>
     <row r="31">
-      <c r="A31" s="38"/>
-      <c r="B31" s="38"/>
+      <c r="A31" s="39"/>
+      <c r="B31" s="39"/>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
@@ -35004,8 +35012,8 @@
       <c r="M31" s="4"/>
     </row>
     <row r="32">
-      <c r="A32" s="38"/>
-      <c r="B32" s="38"/>
+      <c r="A32" s="39"/>
+      <c r="B32" s="39"/>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
@@ -35019,8 +35027,8 @@
       <c r="M32" s="4"/>
     </row>
     <row r="33">
-      <c r="A33" s="38"/>
-      <c r="B33" s="38"/>
+      <c r="A33" s="39"/>
+      <c r="B33" s="39"/>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
@@ -35034,8 +35042,8 @@
       <c r="M33" s="4"/>
     </row>
     <row r="34">
-      <c r="A34" s="38"/>
-      <c r="B34" s="38"/>
+      <c r="A34" s="39"/>
+      <c r="B34" s="39"/>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
@@ -35049,8 +35057,8 @@
       <c r="M34" s="4"/>
     </row>
     <row r="35">
-      <c r="A35" s="38"/>
-      <c r="B35" s="38"/>
+      <c r="A35" s="39"/>
+      <c r="B35" s="39"/>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
@@ -35064,8 +35072,8 @@
       <c r="M35" s="4"/>
     </row>
     <row r="36">
-      <c r="A36" s="38"/>
-      <c r="B36" s="38"/>
+      <c r="A36" s="39"/>
+      <c r="B36" s="39"/>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
@@ -35079,8 +35087,8 @@
       <c r="M36" s="4"/>
     </row>
     <row r="37">
-      <c r="A37" s="38"/>
-      <c r="B37" s="38"/>
+      <c r="A37" s="39"/>
+      <c r="B37" s="39"/>
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
@@ -35094,8 +35102,8 @@
       <c r="M37" s="4"/>
     </row>
     <row r="38">
-      <c r="A38" s="38"/>
-      <c r="B38" s="38"/>
+      <c r="A38" s="39"/>
+      <c r="B38" s="39"/>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
@@ -35109,8 +35117,8 @@
       <c r="M38" s="4"/>
     </row>
     <row r="39">
-      <c r="A39" s="38"/>
-      <c r="B39" s="38"/>
+      <c r="A39" s="39"/>
+      <c r="B39" s="39"/>
       <c r="C39" s="4"/>
       <c r="D39" s="4"/>
       <c r="E39" s="4"/>
@@ -35124,8 +35132,8 @@
       <c r="M39" s="4"/>
     </row>
     <row r="40">
-      <c r="A40" s="38"/>
-      <c r="B40" s="38"/>
+      <c r="A40" s="39"/>
+      <c r="B40" s="39"/>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
@@ -35139,8 +35147,8 @@
       <c r="M40" s="4"/>
     </row>
     <row r="41">
-      <c r="A41" s="38"/>
-      <c r="B41" s="38"/>
+      <c r="A41" s="39"/>
+      <c r="B41" s="39"/>
       <c r="C41" s="4"/>
       <c r="D41" s="4"/>
       <c r="E41" s="4"/>
@@ -35154,8 +35162,8 @@
       <c r="M41" s="4"/>
     </row>
     <row r="42">
-      <c r="A42" s="38"/>
-      <c r="B42" s="38"/>
+      <c r="A42" s="39"/>
+      <c r="B42" s="39"/>
       <c r="C42" s="4"/>
       <c r="D42" s="4"/>
       <c r="E42" s="4"/>
@@ -35169,8 +35177,8 @@
       <c r="M42" s="4"/>
     </row>
     <row r="43">
-      <c r="A43" s="38"/>
-      <c r="B43" s="38"/>
+      <c r="A43" s="39"/>
+      <c r="B43" s="39"/>
       <c r="C43" s="4"/>
       <c r="D43" s="4"/>
       <c r="E43" s="4"/>
@@ -35184,8 +35192,8 @@
       <c r="M43" s="4"/>
     </row>
     <row r="44">
-      <c r="A44" s="38"/>
-      <c r="B44" s="38"/>
+      <c r="A44" s="39"/>
+      <c r="B44" s="39"/>
       <c r="C44" s="4"/>
       <c r="D44" s="4"/>
       <c r="E44" s="4"/>
@@ -35199,8 +35207,8 @@
       <c r="M44" s="4"/>
     </row>
     <row r="45">
-      <c r="A45" s="38"/>
-      <c r="B45" s="38"/>
+      <c r="A45" s="39"/>
+      <c r="B45" s="39"/>
       <c r="C45" s="4"/>
       <c r="D45" s="4"/>
       <c r="E45" s="4"/>
@@ -35214,8 +35222,8 @@
       <c r="M45" s="4"/>
     </row>
     <row r="46">
-      <c r="A46" s="38"/>
-      <c r="B46" s="38"/>
+      <c r="A46" s="39"/>
+      <c r="B46" s="39"/>
       <c r="C46" s="4"/>
       <c r="D46" s="4"/>
       <c r="E46" s="4"/>

</xml_diff>

<commit_message>
Update Laser.xlsx from Google Sheets @ 2025-12-18T10:48:09.265Z
</commit_message>
<xml_diff>
--- a/Laser.xlsx
+++ b/Laser.xlsx
@@ -34968,8 +34968,12 @@
       <c r="A29" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="B29" s="39"/>
-      <c r="C29" s="4"/>
+      <c r="B29" s="38">
+        <v>100.0</v>
+      </c>
+      <c r="C29" s="15">
+        <v>1.0</v>
+      </c>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>

</xml_diff>

<commit_message>
Update Laser.xlsx from Google Sheets @ 2025-12-18T10:48:10.276Z
</commit_message>
<xml_diff>
--- a/Laser.xlsx
+++ b/Laser.xlsx
@@ -223,7 +223,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -337,6 +337,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="14" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -34975,7 +34978,9 @@
         <v>1.0</v>
       </c>
       <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
+      <c r="E29" s="39">
+        <v>46009.78341685185</v>
+      </c>
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
@@ -34986,8 +34991,8 @@
       <c r="M29" s="4"/>
     </row>
     <row r="30">
-      <c r="A30" s="39"/>
-      <c r="B30" s="39"/>
+      <c r="A30" s="40"/>
+      <c r="B30" s="40"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
@@ -35001,8 +35006,8 @@
       <c r="M30" s="4"/>
     </row>
     <row r="31">
-      <c r="A31" s="39"/>
-      <c r="B31" s="39"/>
+      <c r="A31" s="40"/>
+      <c r="B31" s="40"/>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
@@ -35016,8 +35021,8 @@
       <c r="M31" s="4"/>
     </row>
     <row r="32">
-      <c r="A32" s="39"/>
-      <c r="B32" s="39"/>
+      <c r="A32" s="40"/>
+      <c r="B32" s="40"/>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
@@ -35031,8 +35036,8 @@
       <c r="M32" s="4"/>
     </row>
     <row r="33">
-      <c r="A33" s="39"/>
-      <c r="B33" s="39"/>
+      <c r="A33" s="40"/>
+      <c r="B33" s="40"/>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
@@ -35046,8 +35051,8 @@
       <c r="M33" s="4"/>
     </row>
     <row r="34">
-      <c r="A34" s="39"/>
-      <c r="B34" s="39"/>
+      <c r="A34" s="40"/>
+      <c r="B34" s="40"/>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
@@ -35061,8 +35066,8 @@
       <c r="M34" s="4"/>
     </row>
     <row r="35">
-      <c r="A35" s="39"/>
-      <c r="B35" s="39"/>
+      <c r="A35" s="40"/>
+      <c r="B35" s="40"/>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
@@ -35076,8 +35081,8 @@
       <c r="M35" s="4"/>
     </row>
     <row r="36">
-      <c r="A36" s="39"/>
-      <c r="B36" s="39"/>
+      <c r="A36" s="40"/>
+      <c r="B36" s="40"/>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
@@ -35091,8 +35096,8 @@
       <c r="M36" s="4"/>
     </row>
     <row r="37">
-      <c r="A37" s="39"/>
-      <c r="B37" s="39"/>
+      <c r="A37" s="40"/>
+      <c r="B37" s="40"/>
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
@@ -35106,8 +35111,8 @@
       <c r="M37" s="4"/>
     </row>
     <row r="38">
-      <c r="A38" s="39"/>
-      <c r="B38" s="39"/>
+      <c r="A38" s="40"/>
+      <c r="B38" s="40"/>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
@@ -35121,8 +35126,8 @@
       <c r="M38" s="4"/>
     </row>
     <row r="39">
-      <c r="A39" s="39"/>
-      <c r="B39" s="39"/>
+      <c r="A39" s="40"/>
+      <c r="B39" s="40"/>
       <c r="C39" s="4"/>
       <c r="D39" s="4"/>
       <c r="E39" s="4"/>
@@ -35136,8 +35141,8 @@
       <c r="M39" s="4"/>
     </row>
     <row r="40">
-      <c r="A40" s="39"/>
-      <c r="B40" s="39"/>
+      <c r="A40" s="40"/>
+      <c r="B40" s="40"/>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
@@ -35151,8 +35156,8 @@
       <c r="M40" s="4"/>
     </row>
     <row r="41">
-      <c r="A41" s="39"/>
-      <c r="B41" s="39"/>
+      <c r="A41" s="40"/>
+      <c r="B41" s="40"/>
       <c r="C41" s="4"/>
       <c r="D41" s="4"/>
       <c r="E41" s="4"/>
@@ -35166,8 +35171,8 @@
       <c r="M41" s="4"/>
     </row>
     <row r="42">
-      <c r="A42" s="39"/>
-      <c r="B42" s="39"/>
+      <c r="A42" s="40"/>
+      <c r="B42" s="40"/>
       <c r="C42" s="4"/>
       <c r="D42" s="4"/>
       <c r="E42" s="4"/>
@@ -35181,8 +35186,8 @@
       <c r="M42" s="4"/>
     </row>
     <row r="43">
-      <c r="A43" s="39"/>
-      <c r="B43" s="39"/>
+      <c r="A43" s="40"/>
+      <c r="B43" s="40"/>
       <c r="C43" s="4"/>
       <c r="D43" s="4"/>
       <c r="E43" s="4"/>
@@ -35196,8 +35201,8 @@
       <c r="M43" s="4"/>
     </row>
     <row r="44">
-      <c r="A44" s="39"/>
-      <c r="B44" s="39"/>
+      <c r="A44" s="40"/>
+      <c r="B44" s="40"/>
       <c r="C44" s="4"/>
       <c r="D44" s="4"/>
       <c r="E44" s="4"/>
@@ -35211,8 +35216,8 @@
       <c r="M44" s="4"/>
     </row>
     <row r="45">
-      <c r="A45" s="39"/>
-      <c r="B45" s="39"/>
+      <c r="A45" s="40"/>
+      <c r="B45" s="40"/>
       <c r="C45" s="4"/>
       <c r="D45" s="4"/>
       <c r="E45" s="4"/>
@@ -35226,8 +35231,8 @@
       <c r="M45" s="4"/>
     </row>
     <row r="46">
-      <c r="A46" s="39"/>
-      <c r="B46" s="39"/>
+      <c r="A46" s="40"/>
+      <c r="B46" s="40"/>
       <c r="C46" s="4"/>
       <c r="D46" s="4"/>
       <c r="E46" s="4"/>

</xml_diff>

<commit_message>
Update Laser.xlsx from Google Sheets @ 2025-12-18T10:48:16.113Z
</commit_message>
<xml_diff>
--- a/Laser.xlsx
+++ b/Laser.xlsx
@@ -34977,9 +34977,11 @@
       <c r="C29" s="15">
         <v>1.0</v>
       </c>
-      <c r="D29" s="4"/>
+      <c r="D29" s="15">
+        <v>2.0</v>
+      </c>
       <c r="E29" s="39">
-        <v>46009.78341685185</v>
+        <v>46009.783484375</v>
       </c>
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>

</xml_diff>

<commit_message>
Update Laser.xlsx from Google Sheets @ 2025-12-18T14:57:14.485Z
</commit_message>
<xml_diff>
--- a/Laser.xlsx
+++ b/Laser.xlsx
@@ -34583,15 +34583,17 @@
         <v>6</v>
       </c>
       <c r="B10" s="30">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
       <c r="C10" s="30">
-        <v>20.0</v>
+        <v>15.0</v>
       </c>
       <c r="D10" s="8">
         <v>1.0</v>
       </c>
-      <c r="E10" s="23"/>
+      <c r="E10" s="24">
+        <v>46009.956378483796</v>
+      </c>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>

</xml_diff>

<commit_message>
Update Laser.xlsx from Google Sheets @ 2026-01-09T12:16:54.662Z
</commit_message>
<xml_diff>
--- a/Laser.xlsx
+++ b/Laser.xlsx
@@ -17173,16 +17173,16 @@
         <v>7</v>
       </c>
       <c r="B11" s="11">
-        <v>23.0</v>
+        <v>25.0</v>
       </c>
       <c r="C11" s="11">
-        <v>3.0</v>
+        <v>10.0</v>
       </c>
       <c r="D11" s="11">
         <v>1.0</v>
       </c>
       <c r="E11" s="25">
-        <v>45900.487762268516</v>
+        <v>46031.84505053241</v>
       </c>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>

</xml_diff>

<commit_message>
Update Laser.xlsx from Google Sheets @ 2026-01-14T16:02:24.792Z
</commit_message>
<xml_diff>
--- a/Laser.xlsx
+++ b/Laser.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Lasercut 2 " sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Lasercut 3" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="XTool P2" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="Lasercut 2 " sheetId="1" r:id="rId5"/>
+    <sheet state="visible" name="Lasercut 3" sheetId="2" r:id="rId6"/>
+    <sheet state="visible" name="XTool P2" sheetId="3" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -365,6 +365,10 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<x18tc:personList xmlns:x18tc="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
   <a:themeElements>
@@ -16991,15 +16995,17 @@
         <v>6</v>
       </c>
       <c r="B3" s="8">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="C3" s="8">
-        <v>15.0</v>
+        <v>20.0</v>
       </c>
       <c r="D3" s="8">
         <v>1.0</v>
       </c>
-      <c r="E3" s="23"/>
+      <c r="E3" s="24">
+        <v>46037.00163333333</v>
+      </c>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>

</xml_diff>

<commit_message>
Update Laser.xlsx from Google Sheets @ 2026-01-16T02:32:07.134Z
</commit_message>
<xml_diff>
--- a/Laser.xlsx
+++ b/Laser.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="27">
   <si>
     <t>項目</t>
   </si>
@@ -17004,7 +17004,7 @@
         <v>1.0</v>
       </c>
       <c r="E3" s="24">
-        <v>46037.00163333333</v>
+        <v>46037.00168581019</v>
       </c>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
@@ -34795,7 +34795,9 @@
       <c r="M19" s="4"/>
     </row>
     <row r="20">
-      <c r="A20" s="16"/>
+      <c r="A20" s="7" t="s">
+        <v>6</v>
+      </c>
       <c r="B20" s="17"/>
       <c r="C20" s="17"/>
       <c r="D20" s="17"/>

</xml_diff>

<commit_message>
Update Laser.xlsx from Google Sheets @ 2026-01-16T02:32:10.747Z
</commit_message>
<xml_diff>
--- a/Laser.xlsx
+++ b/Laser.xlsx
@@ -34798,7 +34798,9 @@
       <c r="A20" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B20" s="17"/>
+      <c r="B20" s="8">
+        <v>10.0</v>
+      </c>
       <c r="C20" s="17"/>
       <c r="D20" s="17"/>
       <c r="E20" s="23"/>

</xml_diff>

<commit_message>
Update Laser.xlsx from Google Sheets @ 2026-01-16T02:32:15.665Z
</commit_message>
<xml_diff>
--- a/Laser.xlsx
+++ b/Laser.xlsx
@@ -34801,9 +34801,15 @@
       <c r="B20" s="8">
         <v>10.0</v>
       </c>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="23"/>
+      <c r="C20" s="8">
+        <v>250.0</v>
+      </c>
+      <c r="D20" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="E20" s="24">
+        <v>46038.4390540625</v>
+      </c>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>

</xml_diff>

<commit_message>
Update Laser.xlsx from Google Sheets @ 2026-01-16T02:33:09.972Z
</commit_message>
<xml_diff>
--- a/Laser.xlsx
+++ b/Laser.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="28">
   <si>
     <t>項目</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>６</t>
+  </si>
+  <si>
+    <t>吉翁號刻線參數</t>
   </si>
   <si>
     <t>5mm</t>
@@ -34810,7 +34813,9 @@
       <c r="E20" s="24">
         <v>46038.439073761576</v>
       </c>
-      <c r="F20" s="4"/>
+      <c r="F20" s="15" t="s">
+        <v>21</v>
+      </c>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
@@ -34821,7 +34826,7 @@
     </row>
     <row r="21">
       <c r="A21" s="34" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B21" s="17"/>
       <c r="C21" s="17"/>
@@ -34838,7 +34843,7 @@
     </row>
     <row r="22">
       <c r="A22" s="7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B22" s="30">
         <v>2.0</v>
@@ -34928,10 +34933,10 @@
     </row>
     <row r="26">
       <c r="A26" s="7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
@@ -34970,7 +34975,7 @@
     </row>
     <row r="28">
       <c r="A28" s="35" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B28" s="36"/>
       <c r="C28" s="36"/>
@@ -34987,7 +34992,7 @@
     </row>
     <row r="29">
       <c r="A29" s="38" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B29" s="38">
         <v>100.0</v>

</xml_diff>

<commit_message>
Update Laser.xlsx from Google Sheets @ 2026-01-16T14:56:20.176Z
</commit_message>
<xml_diff>
--- a/Laser.xlsx
+++ b/Laser.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="29">
   <si>
     <t>項目</t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>Cut1-2</t>
+  </si>
+  <si>
+    <t>柔光板</t>
   </si>
 </sst>
 </file>
@@ -35031,7 +35034,9 @@
       <c r="M30" s="4"/>
     </row>
     <row r="31">
-      <c r="A31" s="40"/>
+      <c r="A31" s="38" t="s">
+        <v>28</v>
+      </c>
       <c r="B31" s="40"/>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>

</xml_diff>

<commit_message>
Update Laser.xlsx from Google Sheets @ 2026-01-16T14:56:28.846Z
</commit_message>
<xml_diff>
--- a/Laser.xlsx
+++ b/Laser.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="29">
   <si>
     <t>項目</t>
   </si>
@@ -35051,7 +35051,9 @@
       <c r="M31" s="4"/>
     </row>
     <row r="32">
-      <c r="A32" s="40"/>
+      <c r="A32" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="B32" s="40"/>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>

</xml_diff>

<commit_message>
Update Laser.xlsx from Google Sheets @ 2026-01-16T14:56:35.558Z
</commit_message>
<xml_diff>
--- a/Laser.xlsx
+++ b/Laser.xlsx
@@ -35054,10 +35054,18 @@
       <c r="A32" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B32" s="40"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
+      <c r="B32" s="38">
+        <v>50.0</v>
+      </c>
+      <c r="C32" s="15">
+        <v>20.0</v>
+      </c>
+      <c r="D32" s="15">
+        <v>1.0</v>
+      </c>
+      <c r="E32" s="39">
+        <v>46038.95590822917</v>
+      </c>
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
       <c r="H32" s="4"/>

</xml_diff>

<commit_message>
Update Laser.xlsx from Google Sheets @ 2026-01-20T14:04:58.535Z
</commit_message>
<xml_diff>
--- a/Laser.xlsx
+++ b/Laser.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="30">
   <si>
     <t>項目</t>
   </si>
@@ -100,6 +100,9 @@
   </si>
   <si>
     <t>柔光板</t>
+  </si>
+  <si>
+    <t>紙</t>
   </si>
 </sst>
 </file>
@@ -35076,7 +35079,9 @@
       <c r="M32" s="4"/>
     </row>
     <row r="33">
-      <c r="A33" s="40"/>
+      <c r="A33" s="38" t="s">
+        <v>29</v>
+      </c>
       <c r="B33" s="40"/>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>

</xml_diff>

<commit_message>
Update Laser.xlsx from Google Sheets @ 2026-01-20T14:05:14.032Z
</commit_message>
<xml_diff>
--- a/Laser.xlsx
+++ b/Laser.xlsx
@@ -35082,10 +35082,16 @@
       <c r="A33" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="B33" s="40"/>
-      <c r="C33" s="4"/>
+      <c r="B33" s="38">
+        <v>3.0</v>
+      </c>
+      <c r="C33" s="15">
+        <v>80.0</v>
+      </c>
       <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
+      <c r="E33" s="39">
+        <v>46042.92027434028</v>
+      </c>
       <c r="F33" s="4"/>
       <c r="G33" s="4"/>
       <c r="H33" s="4"/>

</xml_diff>

<commit_message>
Update Laser.xlsx from Google Sheets @ 2026-01-21T05:19:39.803Z
</commit_message>
<xml_diff>
--- a/Laser.xlsx
+++ b/Laser.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="31">
   <si>
     <t>項目</t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t>Fill</t>
+  </si>
+  <si>
+    <t>甲板紙</t>
   </si>
   <si>
     <t>遮蓋膠紙</t>
@@ -17669,7 +17672,9 @@
       <c r="O32" s="4"/>
     </row>
     <row r="33">
-      <c r="A33" s="4"/>
+      <c r="A33" s="15" t="s">
+        <v>16</v>
+      </c>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
@@ -17686,7 +17691,9 @@
       <c r="O33" s="4"/>
     </row>
     <row r="34">
-      <c r="A34" s="4"/>
+      <c r="A34" s="15">
+        <v>5.0</v>
+      </c>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
@@ -34416,10 +34423,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
@@ -34496,7 +34503,7 @@
     </row>
     <row r="5">
       <c r="A5" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
@@ -34538,7 +34545,7 @@
     </row>
     <row r="7">
       <c r="A7" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B7" s="8">
         <v>20.0</v>
@@ -34678,7 +34685,7 @@
         <v>6</v>
       </c>
       <c r="B14" s="33" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C14" s="33">
         <v>20.0</v>
@@ -34820,7 +34827,7 @@
         <v>46038.439073761576</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
@@ -34832,7 +34839,7 @@
     </row>
     <row r="21">
       <c r="A21" s="34" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B21" s="17"/>
       <c r="C21" s="17"/>
@@ -34849,7 +34856,7 @@
     </row>
     <row r="22">
       <c r="A22" s="7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B22" s="30">
         <v>2.0</v>
@@ -34939,10 +34946,10 @@
     </row>
     <row r="26">
       <c r="A26" s="7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
@@ -34981,7 +34988,7 @@
     </row>
     <row r="28">
       <c r="A28" s="35" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B28" s="36"/>
       <c r="C28" s="36"/>
@@ -34998,7 +35005,7 @@
     </row>
     <row r="29">
       <c r="A29" s="38" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B29" s="38">
         <v>100.0</v>
@@ -35038,7 +35045,7 @@
     </row>
     <row r="31">
       <c r="A31" s="38" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B31" s="40"/>
       <c r="C31" s="4"/>
@@ -35080,7 +35087,7 @@
     </row>
     <row r="33">
       <c r="A33" s="38" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B33" s="38">
         <v>3.0</v>

</xml_diff>

<commit_message>
Update Laser.xlsx from Google Sheets @ 2026-01-21T05:19:44.482Z
</commit_message>
<xml_diff>
--- a/Laser.xlsx
+++ b/Laser.xlsx
@@ -324,6 +324,9 @@
     <xf borderId="8" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="14" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
@@ -349,9 +352,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="14" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -17694,10 +17694,14 @@
       <c r="A34" s="15">
         <v>5.0</v>
       </c>
-      <c r="B34" s="4"/>
+      <c r="B34" s="15">
+        <v>10.0</v>
+      </c>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
+      <c r="E34" s="30">
+        <v>46043.555360555554</v>
+      </c>
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
@@ -34450,8 +34454,8 @@
       <c r="A2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
       <c r="D2" s="8"/>
       <c r="E2" s="23"/>
       <c r="F2" s="4"/>
@@ -34467,10 +34471,10 @@
       <c r="A3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="30">
+      <c r="B3" s="31">
         <v>60.0</v>
       </c>
-      <c r="C3" s="30">
+      <c r="C3" s="31">
         <v>20.0</v>
       </c>
       <c r="D3" s="8">
@@ -34570,10 +34574,10 @@
     </row>
     <row r="8">
       <c r="A8" s="5"/>
-      <c r="B8" s="31"/>
-      <c r="C8" s="31"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="32"/>
+      <c r="B8" s="32"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="33"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
@@ -34604,10 +34608,10 @@
       <c r="A10" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="30">
+      <c r="B10" s="31">
         <v>4.0</v>
       </c>
-      <c r="C10" s="30">
+      <c r="C10" s="31">
         <v>15.0</v>
       </c>
       <c r="D10" s="8">
@@ -34629,10 +34633,10 @@
       <c r="A11" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="30">
+      <c r="B11" s="31">
         <v>18.0</v>
       </c>
-      <c r="C11" s="30">
+      <c r="C11" s="31">
         <v>15.0</v>
       </c>
       <c r="D11" s="8">
@@ -34684,13 +34688,13 @@
       <c r="A14" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="33" t="s">
+      <c r="B14" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="33">
+      <c r="C14" s="34">
         <v>20.0</v>
       </c>
-      <c r="D14" s="33">
+      <c r="D14" s="34">
         <v>1.0</v>
       </c>
       <c r="E14" s="25">
@@ -34709,13 +34713,13 @@
       <c r="A15" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B15" s="33">
+      <c r="B15" s="34">
         <v>30.0</v>
       </c>
-      <c r="C15" s="33">
+      <c r="C15" s="34">
         <v>15.0</v>
       </c>
-      <c r="D15" s="33">
+      <c r="D15" s="34">
         <v>1.0</v>
       </c>
       <c r="E15" s="26"/>
@@ -34838,7 +34842,7 @@
       <c r="M20" s="4"/>
     </row>
     <row r="21">
-      <c r="A21" s="34" t="s">
+      <c r="A21" s="35" t="s">
         <v>23</v>
       </c>
       <c r="B21" s="17"/>
@@ -34858,13 +34862,13 @@
       <c r="A22" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="30">
+      <c r="B22" s="31">
         <v>2.0</v>
       </c>
-      <c r="C22" s="30">
+      <c r="C22" s="31">
         <v>100.0</v>
       </c>
-      <c r="D22" s="30">
+      <c r="D22" s="31">
         <v>1.0</v>
       </c>
       <c r="E22" s="24">
@@ -34883,13 +34887,13 @@
       <c r="A23" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B23" s="30">
+      <c r="B23" s="31">
         <v>2.0</v>
       </c>
-      <c r="C23" s="30">
+      <c r="C23" s="31">
         <v>85.0</v>
       </c>
-      <c r="D23" s="30">
+      <c r="D23" s="31">
         <v>1.0</v>
       </c>
       <c r="E23" s="24">
@@ -34908,13 +34912,13 @@
       <c r="A24" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B24" s="30">
+      <c r="B24" s="31">
         <v>70.0</v>
       </c>
-      <c r="C24" s="30">
+      <c r="C24" s="31">
         <v>10.0</v>
       </c>
-      <c r="D24" s="30">
+      <c r="D24" s="31">
         <v>1.0</v>
       </c>
       <c r="E24" s="24">
@@ -34987,13 +34991,13 @@
       <c r="M27" s="4"/>
     </row>
     <row r="28">
-      <c r="A28" s="35" t="s">
+      <c r="A28" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="36"/>
-      <c r="C28" s="36"/>
-      <c r="D28" s="36"/>
-      <c r="E28" s="37"/>
+      <c r="B28" s="37"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="38"/>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
@@ -35004,10 +35008,10 @@
       <c r="M28" s="4"/>
     </row>
     <row r="29">
-      <c r="A29" s="38" t="s">
+      <c r="A29" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="38">
+      <c r="B29" s="39">
         <v>100.0</v>
       </c>
       <c r="C29" s="15">
@@ -35016,7 +35020,7 @@
       <c r="D29" s="15">
         <v>2.0</v>
       </c>
-      <c r="E29" s="39">
+      <c r="E29" s="30">
         <v>46009.783484375</v>
       </c>
       <c r="F29" s="4"/>
@@ -35044,7 +35048,7 @@
       <c r="M30" s="4"/>
     </row>
     <row r="31">
-      <c r="A31" s="38" t="s">
+      <c r="A31" s="39" t="s">
         <v>29</v>
       </c>
       <c r="B31" s="40"/>
@@ -35064,7 +35068,7 @@
       <c r="A32" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B32" s="38">
+      <c r="B32" s="39">
         <v>50.0</v>
       </c>
       <c r="C32" s="15">
@@ -35073,7 +35077,7 @@
       <c r="D32" s="15">
         <v>1.0</v>
       </c>
-      <c r="E32" s="39">
+      <c r="E32" s="30">
         <v>46038.9559609375</v>
       </c>
       <c r="F32" s="4"/>
@@ -35086,17 +35090,17 @@
       <c r="M32" s="4"/>
     </row>
     <row r="33">
-      <c r="A33" s="38" t="s">
+      <c r="A33" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="B33" s="38">
+      <c r="B33" s="39">
         <v>3.0</v>
       </c>
       <c r="C33" s="15">
         <v>80.0</v>
       </c>
       <c r="D33" s="4"/>
-      <c r="E33" s="39">
+      <c r="E33" s="30">
         <v>46042.92027434028</v>
       </c>
       <c r="F33" s="4"/>

</xml_diff>

<commit_message>
Update Laser.xlsx from Google Sheets @ 2026-01-21T05:19:48.206Z
</commit_message>
<xml_diff>
--- a/Laser.xlsx
+++ b/Laser.xlsx
@@ -17691,11 +17691,9 @@
       <c r="O33" s="4"/>
     </row>
     <row r="34">
-      <c r="A34" s="15">
+      <c r="A34" s="15"/>
+      <c r="B34" s="15">
         <v>5.0</v>
-      </c>
-      <c r="B34" s="15">
-        <v>10.0</v>
       </c>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>

</xml_diff>

<commit_message>
Update Laser.xlsx from Google Sheets @ 2026-01-21T05:19:50.449Z
</commit_message>
<xml_diff>
--- a/Laser.xlsx
+++ b/Laser.xlsx
@@ -17695,10 +17695,14 @@
       <c r="B34" s="15">
         <v>5.0</v>
       </c>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
+      <c r="C34" s="15">
+        <v>10.0</v>
+      </c>
+      <c r="D34" s="15">
+        <v>2.0</v>
+      </c>
       <c r="E34" s="30">
-        <v>46043.555360555554</v>
+        <v>46043.55542802083</v>
       </c>
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>

</xml_diff>

<commit_message>
Update Laser.xlsx from Google Sheets @ 2026-01-21T05:19:52.017Z
</commit_message>
<xml_diff>
--- a/Laser.xlsx
+++ b/Laser.xlsx
@@ -17672,9 +17672,6 @@
       <c r="O32" s="4"/>
     </row>
     <row r="33">
-      <c r="A33" s="15" t="s">
-        <v>16</v>
-      </c>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
@@ -17691,7 +17688,9 @@
       <c r="O33" s="4"/>
     </row>
     <row r="34">
-      <c r="A34" s="15"/>
+      <c r="A34" s="15" t="s">
+        <v>16</v>
+      </c>
       <c r="B34" s="15">
         <v>5.0</v>
       </c>

</xml_diff>

<commit_message>
Update Laser.xlsx from Google Sheets @ 2026-01-21T05:20:07.923Z
</commit_message>
<xml_diff>
--- a/Laser.xlsx
+++ b/Laser.xlsx
@@ -17671,11 +17671,22 @@
       <c r="N32" s="4"/>
       <c r="O32" s="4"/>
     </row>
-    <row r="33">
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
+    <row r="33" ht="20.25" customHeight="1">
+      <c r="A33" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B33" s="15">
+        <v>5.0</v>
+      </c>
+      <c r="C33" s="15">
+        <v>10.0</v>
+      </c>
+      <c r="D33" s="15">
+        <v>2.0</v>
+      </c>
+      <c r="E33" s="30">
+        <v>46043.55545597222</v>
+      </c>
       <c r="F33" s="4"/>
       <c r="G33" s="4"/>
       <c r="H33" s="4"/>
@@ -17687,22 +17698,12 @@
       <c r="N33" s="4"/>
       <c r="O33" s="4"/>
     </row>
-    <row r="34" ht="20.25" customHeight="1">
-      <c r="A34" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="B34" s="15">
-        <v>5.0</v>
-      </c>
-      <c r="C34" s="15">
-        <v>10.0</v>
-      </c>
-      <c r="D34" s="15">
-        <v>2.0</v>
-      </c>
-      <c r="E34" s="30">
-        <v>46043.55545597222</v>
-      </c>
+    <row r="34">
+      <c r="A34" s="4"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
@@ -34390,23 +34391,6 @@
       <c r="M1015" s="4"/>
       <c r="N1015" s="4"/>
       <c r="O1015" s="4"/>
-    </row>
-    <row r="1016">
-      <c r="A1016" s="4"/>
-      <c r="B1016" s="4"/>
-      <c r="C1016" s="4"/>
-      <c r="D1016" s="4"/>
-      <c r="E1016" s="4"/>
-      <c r="F1016" s="4"/>
-      <c r="G1016" s="4"/>
-      <c r="H1016" s="4"/>
-      <c r="I1016" s="4"/>
-      <c r="J1016" s="4"/>
-      <c r="K1016" s="4"/>
-      <c r="L1016" s="4"/>
-      <c r="M1016" s="4"/>
-      <c r="N1016" s="4"/>
-      <c r="O1016" s="4"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Update Laser.xlsx from Google Sheets @ 2026-01-21T05:20:16.213Z
</commit_message>
<xml_diff>
--- a/Laser.xlsx
+++ b/Laser.xlsx
@@ -177,7 +177,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="12">
     <border/>
     <border>
       <left style="thin">
@@ -231,11 +231,41 @@
         <color rgb="FF000000"/>
       </bottom>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="44">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -324,7 +354,13 @@
     <xf borderId="8" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="14" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="9" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="10" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="11" fillId="0" fontId="2" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -352,6 +388,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="14" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -17672,19 +17711,19 @@
       <c r="O32" s="4"/>
     </row>
     <row r="33" ht="20.25" customHeight="1">
-      <c r="A33" s="15" t="s">
+      <c r="A33" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="B33" s="15">
+      <c r="B33" s="31">
         <v>5.0</v>
       </c>
-      <c r="C33" s="15">
+      <c r="C33" s="31">
         <v>10.0</v>
       </c>
-      <c r="D33" s="15">
+      <c r="D33" s="31">
         <v>2.0</v>
       </c>
-      <c r="E33" s="30">
+      <c r="E33" s="32">
         <v>46043.55545597222</v>
       </c>
       <c r="F33" s="4"/>
@@ -34439,8 +34478,8 @@
       <c r="A2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
       <c r="D2" s="8"/>
       <c r="E2" s="23"/>
       <c r="F2" s="4"/>
@@ -34456,10 +34495,10 @@
       <c r="A3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="31">
+      <c r="B3" s="33">
         <v>60.0</v>
       </c>
-      <c r="C3" s="31">
+      <c r="C3" s="33">
         <v>20.0</v>
       </c>
       <c r="D3" s="8">
@@ -34559,10 +34598,10 @@
     </row>
     <row r="8">
       <c r="A8" s="5"/>
-      <c r="B8" s="32"/>
-      <c r="C8" s="32"/>
-      <c r="D8" s="32"/>
-      <c r="E8" s="33"/>
+      <c r="B8" s="34"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="35"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
@@ -34593,10 +34632,10 @@
       <c r="A10" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="31">
+      <c r="B10" s="33">
         <v>4.0</v>
       </c>
-      <c r="C10" s="31">
+      <c r="C10" s="33">
         <v>15.0</v>
       </c>
       <c r="D10" s="8">
@@ -34618,10 +34657,10 @@
       <c r="A11" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="31">
+      <c r="B11" s="33">
         <v>18.0</v>
       </c>
-      <c r="C11" s="31">
+      <c r="C11" s="33">
         <v>15.0</v>
       </c>
       <c r="D11" s="8">
@@ -34673,13 +34712,13 @@
       <c r="A14" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="34" t="s">
+      <c r="B14" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="34">
+      <c r="C14" s="36">
         <v>20.0</v>
       </c>
-      <c r="D14" s="34">
+      <c r="D14" s="36">
         <v>1.0</v>
       </c>
       <c r="E14" s="25">
@@ -34698,13 +34737,13 @@
       <c r="A15" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B15" s="34">
+      <c r="B15" s="36">
         <v>30.0</v>
       </c>
-      <c r="C15" s="34">
+      <c r="C15" s="36">
         <v>15.0</v>
       </c>
-      <c r="D15" s="34">
+      <c r="D15" s="36">
         <v>1.0</v>
       </c>
       <c r="E15" s="26"/>
@@ -34827,7 +34866,7 @@
       <c r="M20" s="4"/>
     </row>
     <row r="21">
-      <c r="A21" s="35" t="s">
+      <c r="A21" s="37" t="s">
         <v>23</v>
       </c>
       <c r="B21" s="17"/>
@@ -34847,13 +34886,13 @@
       <c r="A22" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="31">
+      <c r="B22" s="33">
         <v>2.0</v>
       </c>
-      <c r="C22" s="31">
+      <c r="C22" s="33">
         <v>100.0</v>
       </c>
-      <c r="D22" s="31">
+      <c r="D22" s="33">
         <v>1.0</v>
       </c>
       <c r="E22" s="24">
@@ -34872,13 +34911,13 @@
       <c r="A23" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B23" s="31">
+      <c r="B23" s="33">
         <v>2.0</v>
       </c>
-      <c r="C23" s="31">
+      <c r="C23" s="33">
         <v>85.0</v>
       </c>
-      <c r="D23" s="31">
+      <c r="D23" s="33">
         <v>1.0</v>
       </c>
       <c r="E23" s="24">
@@ -34897,13 +34936,13 @@
       <c r="A24" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B24" s="31">
+      <c r="B24" s="33">
         <v>70.0</v>
       </c>
-      <c r="C24" s="31">
+      <c r="C24" s="33">
         <v>10.0</v>
       </c>
-      <c r="D24" s="31">
+      <c r="D24" s="33">
         <v>1.0</v>
       </c>
       <c r="E24" s="24">
@@ -34976,13 +35015,13 @@
       <c r="M27" s="4"/>
     </row>
     <row r="28">
-      <c r="A28" s="36" t="s">
+      <c r="A28" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="37"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="38"/>
+      <c r="B28" s="39"/>
+      <c r="C28" s="39"/>
+      <c r="D28" s="39"/>
+      <c r="E28" s="40"/>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
@@ -34993,10 +35032,10 @@
       <c r="M28" s="4"/>
     </row>
     <row r="29">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="39">
+      <c r="B29" s="41">
         <v>100.0</v>
       </c>
       <c r="C29" s="15">
@@ -35005,7 +35044,7 @@
       <c r="D29" s="15">
         <v>2.0</v>
       </c>
-      <c r="E29" s="30">
+      <c r="E29" s="42">
         <v>46009.783484375</v>
       </c>
       <c r="F29" s="4"/>
@@ -35018,8 +35057,8 @@
       <c r="M29" s="4"/>
     </row>
     <row r="30">
-      <c r="A30" s="40"/>
-      <c r="B30" s="40"/>
+      <c r="A30" s="43"/>
+      <c r="B30" s="43"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
@@ -35033,10 +35072,10 @@
       <c r="M30" s="4"/>
     </row>
     <row r="31">
-      <c r="A31" s="39" t="s">
+      <c r="A31" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="40"/>
+      <c r="B31" s="43"/>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
@@ -35053,7 +35092,7 @@
       <c r="A32" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B32" s="39">
+      <c r="B32" s="41">
         <v>50.0</v>
       </c>
       <c r="C32" s="15">
@@ -35062,7 +35101,7 @@
       <c r="D32" s="15">
         <v>1.0</v>
       </c>
-      <c r="E32" s="30">
+      <c r="E32" s="42">
         <v>46038.9559609375</v>
       </c>
       <c r="F32" s="4"/>
@@ -35075,17 +35114,17 @@
       <c r="M32" s="4"/>
     </row>
     <row r="33">
-      <c r="A33" s="39" t="s">
+      <c r="A33" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="B33" s="39">
+      <c r="B33" s="41">
         <v>3.0</v>
       </c>
       <c r="C33" s="15">
         <v>80.0</v>
       </c>
       <c r="D33" s="4"/>
-      <c r="E33" s="30">
+      <c r="E33" s="42">
         <v>46042.92027434028</v>
       </c>
       <c r="F33" s="4"/>
@@ -35098,8 +35137,8 @@
       <c r="M33" s="4"/>
     </row>
     <row r="34">
-      <c r="A34" s="40"/>
-      <c r="B34" s="40"/>
+      <c r="A34" s="43"/>
+      <c r="B34" s="43"/>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
@@ -35113,8 +35152,8 @@
       <c r="M34" s="4"/>
     </row>
     <row r="35">
-      <c r="A35" s="40"/>
-      <c r="B35" s="40"/>
+      <c r="A35" s="43"/>
+      <c r="B35" s="43"/>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
@@ -35128,8 +35167,8 @@
       <c r="M35" s="4"/>
     </row>
     <row r="36">
-      <c r="A36" s="40"/>
-      <c r="B36" s="40"/>
+      <c r="A36" s="43"/>
+      <c r="B36" s="43"/>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
@@ -35143,8 +35182,8 @@
       <c r="M36" s="4"/>
     </row>
     <row r="37">
-      <c r="A37" s="40"/>
-      <c r="B37" s="40"/>
+      <c r="A37" s="43"/>
+      <c r="B37" s="43"/>
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
@@ -35158,8 +35197,8 @@
       <c r="M37" s="4"/>
     </row>
     <row r="38">
-      <c r="A38" s="40"/>
-      <c r="B38" s="40"/>
+      <c r="A38" s="43"/>
+      <c r="B38" s="43"/>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
@@ -35173,8 +35212,8 @@
       <c r="M38" s="4"/>
     </row>
     <row r="39">
-      <c r="A39" s="40"/>
-      <c r="B39" s="40"/>
+      <c r="A39" s="43"/>
+      <c r="B39" s="43"/>
       <c r="C39" s="4"/>
       <c r="D39" s="4"/>
       <c r="E39" s="4"/>
@@ -35188,8 +35227,8 @@
       <c r="M39" s="4"/>
     </row>
     <row r="40">
-      <c r="A40" s="40"/>
-      <c r="B40" s="40"/>
+      <c r="A40" s="43"/>
+      <c r="B40" s="43"/>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
@@ -35203,8 +35242,8 @@
       <c r="M40" s="4"/>
     </row>
     <row r="41">
-      <c r="A41" s="40"/>
-      <c r="B41" s="40"/>
+      <c r="A41" s="43"/>
+      <c r="B41" s="43"/>
       <c r="C41" s="4"/>
       <c r="D41" s="4"/>
       <c r="E41" s="4"/>
@@ -35218,8 +35257,8 @@
       <c r="M41" s="4"/>
     </row>
     <row r="42">
-      <c r="A42" s="40"/>
-      <c r="B42" s="40"/>
+      <c r="A42" s="43"/>
+      <c r="B42" s="43"/>
       <c r="C42" s="4"/>
       <c r="D42" s="4"/>
       <c r="E42" s="4"/>
@@ -35233,8 +35272,8 @@
       <c r="M42" s="4"/>
     </row>
     <row r="43">
-      <c r="A43" s="40"/>
-      <c r="B43" s="40"/>
+      <c r="A43" s="43"/>
+      <c r="B43" s="43"/>
       <c r="C43" s="4"/>
       <c r="D43" s="4"/>
       <c r="E43" s="4"/>
@@ -35248,8 +35287,8 @@
       <c r="M43" s="4"/>
     </row>
     <row r="44">
-      <c r="A44" s="40"/>
-      <c r="B44" s="40"/>
+      <c r="A44" s="43"/>
+      <c r="B44" s="43"/>
       <c r="C44" s="4"/>
       <c r="D44" s="4"/>
       <c r="E44" s="4"/>
@@ -35263,8 +35302,8 @@
       <c r="M44" s="4"/>
     </row>
     <row r="45">
-      <c r="A45" s="40"/>
-      <c r="B45" s="40"/>
+      <c r="A45" s="43"/>
+      <c r="B45" s="43"/>
       <c r="C45" s="4"/>
       <c r="D45" s="4"/>
       <c r="E45" s="4"/>
@@ -35278,8 +35317,8 @@
       <c r="M45" s="4"/>
     </row>
     <row r="46">
-      <c r="A46" s="40"/>
-      <c r="B46" s="40"/>
+      <c r="A46" s="43"/>
+      <c r="B46" s="43"/>
       <c r="C46" s="4"/>
       <c r="D46" s="4"/>
       <c r="E46" s="4"/>

</xml_diff>

<commit_message>
Update Laser.xlsx from Google Sheets @ 2026-01-21T05:20:21.220Z
</commit_message>
<xml_diff>
--- a/Laser.xlsx
+++ b/Laser.xlsx
@@ -138,6 +138,12 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12.0"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="14.0"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -146,12 +152,6 @@
     <font>
       <b/>
       <sz val="14.0"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12.0"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -354,16 +354,19 @@
     <xf borderId="8" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="9" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="9" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="10" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="10" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="11" fillId="0" fontId="2" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="11" fillId="0" fontId="4" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -372,10 +375,10 @@
     <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -387,14 +390,11 @@
     <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="14" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -17726,16 +17726,16 @@
       <c r="E33" s="32">
         <v>46043.55545597222</v>
       </c>
-      <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
-      <c r="H33" s="4"/>
-      <c r="I33" s="4"/>
-      <c r="J33" s="4"/>
-      <c r="K33" s="4"/>
-      <c r="L33" s="4"/>
-      <c r="M33" s="4"/>
-      <c r="N33" s="4"/>
-      <c r="O33" s="4"/>
+      <c r="F33" s="33"/>
+      <c r="G33" s="33"/>
+      <c r="H33" s="33"/>
+      <c r="I33" s="33"/>
+      <c r="J33" s="33"/>
+      <c r="K33" s="33"/>
+      <c r="L33" s="33"/>
+      <c r="M33" s="33"/>
+      <c r="N33" s="33"/>
+      <c r="O33" s="33"/>
     </row>
     <row r="34">
       <c r="A34" s="4"/>
@@ -34478,8 +34478,8 @@
       <c r="A2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
       <c r="D2" s="8"/>
       <c r="E2" s="23"/>
       <c r="F2" s="4"/>
@@ -34495,10 +34495,10 @@
       <c r="A3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="33">
+      <c r="B3" s="34">
         <v>60.0</v>
       </c>
-      <c r="C3" s="33">
+      <c r="C3" s="34">
         <v>20.0</v>
       </c>
       <c r="D3" s="8">
@@ -34598,10 +34598,10 @@
     </row>
     <row r="8">
       <c r="A8" s="5"/>
-      <c r="B8" s="34"/>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="35"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="36"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
@@ -34632,10 +34632,10 @@
       <c r="A10" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="33">
+      <c r="B10" s="34">
         <v>4.0</v>
       </c>
-      <c r="C10" s="33">
+      <c r="C10" s="34">
         <v>15.0</v>
       </c>
       <c r="D10" s="8">
@@ -34657,10 +34657,10 @@
       <c r="A11" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="33">
+      <c r="B11" s="34">
         <v>18.0</v>
       </c>
-      <c r="C11" s="33">
+      <c r="C11" s="34">
         <v>15.0</v>
       </c>
       <c r="D11" s="8">
@@ -34712,13 +34712,13 @@
       <c r="A14" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="36" t="s">
+      <c r="B14" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="36">
+      <c r="C14" s="37">
         <v>20.0</v>
       </c>
-      <c r="D14" s="36">
+      <c r="D14" s="37">
         <v>1.0</v>
       </c>
       <c r="E14" s="25">
@@ -34737,13 +34737,13 @@
       <c r="A15" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B15" s="36">
+      <c r="B15" s="37">
         <v>30.0</v>
       </c>
-      <c r="C15" s="36">
+      <c r="C15" s="37">
         <v>15.0</v>
       </c>
-      <c r="D15" s="36">
+      <c r="D15" s="37">
         <v>1.0</v>
       </c>
       <c r="E15" s="26"/>
@@ -34866,7 +34866,7 @@
       <c r="M20" s="4"/>
     </row>
     <row r="21">
-      <c r="A21" s="37" t="s">
+      <c r="A21" s="38" t="s">
         <v>23</v>
       </c>
       <c r="B21" s="17"/>
@@ -34886,13 +34886,13 @@
       <c r="A22" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="33">
+      <c r="B22" s="34">
         <v>2.0</v>
       </c>
-      <c r="C22" s="33">
+      <c r="C22" s="34">
         <v>100.0</v>
       </c>
-      <c r="D22" s="33">
+      <c r="D22" s="34">
         <v>1.0</v>
       </c>
       <c r="E22" s="24">
@@ -34911,13 +34911,13 @@
       <c r="A23" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B23" s="33">
+      <c r="B23" s="34">
         <v>2.0</v>
       </c>
-      <c r="C23" s="33">
+      <c r="C23" s="34">
         <v>85.0</v>
       </c>
-      <c r="D23" s="33">
+      <c r="D23" s="34">
         <v>1.0</v>
       </c>
       <c r="E23" s="24">
@@ -34936,13 +34936,13 @@
       <c r="A24" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B24" s="33">
+      <c r="B24" s="34">
         <v>70.0</v>
       </c>
-      <c r="C24" s="33">
+      <c r="C24" s="34">
         <v>10.0</v>
       </c>
-      <c r="D24" s="33">
+      <c r="D24" s="34">
         <v>1.0</v>
       </c>
       <c r="E24" s="24">
@@ -35015,13 +35015,13 @@
       <c r="M27" s="4"/>
     </row>
     <row r="28">
-      <c r="A28" s="38" t="s">
+      <c r="A28" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="39"/>
-      <c r="C28" s="39"/>
-      <c r="D28" s="39"/>
-      <c r="E28" s="40"/>
+      <c r="B28" s="40"/>
+      <c r="C28" s="40"/>
+      <c r="D28" s="40"/>
+      <c r="E28" s="41"/>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
@@ -35032,10 +35032,10 @@
       <c r="M28" s="4"/>
     </row>
     <row r="29">
-      <c r="A29" s="41" t="s">
+      <c r="A29" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="41">
+      <c r="B29" s="42">
         <v>100.0</v>
       </c>
       <c r="C29" s="15">
@@ -35044,7 +35044,7 @@
       <c r="D29" s="15">
         <v>2.0</v>
       </c>
-      <c r="E29" s="42">
+      <c r="E29" s="43">
         <v>46009.783484375</v>
       </c>
       <c r="F29" s="4"/>
@@ -35057,8 +35057,8 @@
       <c r="M29" s="4"/>
     </row>
     <row r="30">
-      <c r="A30" s="43"/>
-      <c r="B30" s="43"/>
+      <c r="A30" s="33"/>
+      <c r="B30" s="33"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
@@ -35072,10 +35072,10 @@
       <c r="M30" s="4"/>
     </row>
     <row r="31">
-      <c r="A31" s="41" t="s">
+      <c r="A31" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="43"/>
+      <c r="B31" s="33"/>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
@@ -35092,7 +35092,7 @@
       <c r="A32" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B32" s="41">
+      <c r="B32" s="42">
         <v>50.0</v>
       </c>
       <c r="C32" s="15">
@@ -35101,7 +35101,7 @@
       <c r="D32" s="15">
         <v>1.0</v>
       </c>
-      <c r="E32" s="42">
+      <c r="E32" s="43">
         <v>46038.9559609375</v>
       </c>
       <c r="F32" s="4"/>
@@ -35114,17 +35114,17 @@
       <c r="M32" s="4"/>
     </row>
     <row r="33">
-      <c r="A33" s="41" t="s">
+      <c r="A33" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="B33" s="41">
+      <c r="B33" s="42">
         <v>3.0</v>
       </c>
       <c r="C33" s="15">
         <v>80.0</v>
       </c>
       <c r="D33" s="4"/>
-      <c r="E33" s="42">
+      <c r="E33" s="43">
         <v>46042.92027434028</v>
       </c>
       <c r="F33" s="4"/>
@@ -35137,8 +35137,8 @@
       <c r="M33" s="4"/>
     </row>
     <row r="34">
-      <c r="A34" s="43"/>
-      <c r="B34" s="43"/>
+      <c r="A34" s="33"/>
+      <c r="B34" s="33"/>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
@@ -35152,8 +35152,8 @@
       <c r="M34" s="4"/>
     </row>
     <row r="35">
-      <c r="A35" s="43"/>
-      <c r="B35" s="43"/>
+      <c r="A35" s="33"/>
+      <c r="B35" s="33"/>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
@@ -35167,8 +35167,8 @@
       <c r="M35" s="4"/>
     </row>
     <row r="36">
-      <c r="A36" s="43"/>
-      <c r="B36" s="43"/>
+      <c r="A36" s="33"/>
+      <c r="B36" s="33"/>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
@@ -35182,8 +35182,8 @@
       <c r="M36" s="4"/>
     </row>
     <row r="37">
-      <c r="A37" s="43"/>
-      <c r="B37" s="43"/>
+      <c r="A37" s="33"/>
+      <c r="B37" s="33"/>
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
@@ -35197,8 +35197,8 @@
       <c r="M37" s="4"/>
     </row>
     <row r="38">
-      <c r="A38" s="43"/>
-      <c r="B38" s="43"/>
+      <c r="A38" s="33"/>
+      <c r="B38" s="33"/>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
@@ -35212,8 +35212,8 @@
       <c r="M38" s="4"/>
     </row>
     <row r="39">
-      <c r="A39" s="43"/>
-      <c r="B39" s="43"/>
+      <c r="A39" s="33"/>
+      <c r="B39" s="33"/>
       <c r="C39" s="4"/>
       <c r="D39" s="4"/>
       <c r="E39" s="4"/>
@@ -35227,8 +35227,8 @@
       <c r="M39" s="4"/>
     </row>
     <row r="40">
-      <c r="A40" s="43"/>
-      <c r="B40" s="43"/>
+      <c r="A40" s="33"/>
+      <c r="B40" s="33"/>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
@@ -35242,8 +35242,8 @@
       <c r="M40" s="4"/>
     </row>
     <row r="41">
-      <c r="A41" s="43"/>
-      <c r="B41" s="43"/>
+      <c r="A41" s="33"/>
+      <c r="B41" s="33"/>
       <c r="C41" s="4"/>
       <c r="D41" s="4"/>
       <c r="E41" s="4"/>
@@ -35257,8 +35257,8 @@
       <c r="M41" s="4"/>
     </row>
     <row r="42">
-      <c r="A42" s="43"/>
-      <c r="B42" s="43"/>
+      <c r="A42" s="33"/>
+      <c r="B42" s="33"/>
       <c r="C42" s="4"/>
       <c r="D42" s="4"/>
       <c r="E42" s="4"/>
@@ -35272,8 +35272,8 @@
       <c r="M42" s="4"/>
     </row>
     <row r="43">
-      <c r="A43" s="43"/>
-      <c r="B43" s="43"/>
+      <c r="A43" s="33"/>
+      <c r="B43" s="33"/>
       <c r="C43" s="4"/>
       <c r="D43" s="4"/>
       <c r="E43" s="4"/>
@@ -35287,8 +35287,8 @@
       <c r="M43" s="4"/>
     </row>
     <row r="44">
-      <c r="A44" s="43"/>
-      <c r="B44" s="43"/>
+      <c r="A44" s="33"/>
+      <c r="B44" s="33"/>
       <c r="C44" s="4"/>
       <c r="D44" s="4"/>
       <c r="E44" s="4"/>
@@ -35302,8 +35302,8 @@
       <c r="M44" s="4"/>
     </row>
     <row r="45">
-      <c r="A45" s="43"/>
-      <c r="B45" s="43"/>
+      <c r="A45" s="33"/>
+      <c r="B45" s="33"/>
       <c r="C45" s="4"/>
       <c r="D45" s="4"/>
       <c r="E45" s="4"/>
@@ -35317,8 +35317,8 @@
       <c r="M45" s="4"/>
     </row>
     <row r="46">
-      <c r="A46" s="43"/>
-      <c r="B46" s="43"/>
+      <c r="A46" s="33"/>
+      <c r="B46" s="33"/>
       <c r="C46" s="4"/>
       <c r="D46" s="4"/>
       <c r="E46" s="4"/>

</xml_diff>

<commit_message>
Update Laser.xlsx from Google Sheets @ 2026-01-21T05:20:45.566Z
</commit_message>
<xml_diff>
--- a/Laser.xlsx
+++ b/Laser.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="32">
   <si>
     <t>項目</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>甲板紙</t>
+  </si>
+  <si>
+    <t>反轉cut, 鏡射</t>
   </si>
   <si>
     <t>遮蓋膠紙</t>
@@ -364,6 +367,9 @@
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -389,9 +395,6 @@
     </xf>
     <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="14" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
@@ -17726,16 +17729,18 @@
       <c r="E33" s="32">
         <v>46043.55545597222</v>
       </c>
-      <c r="F33" s="33"/>
-      <c r="G33" s="33"/>
-      <c r="H33" s="33"/>
-      <c r="I33" s="33"/>
-      <c r="J33" s="33"/>
-      <c r="K33" s="33"/>
-      <c r="L33" s="33"/>
-      <c r="M33" s="33"/>
-      <c r="N33" s="33"/>
-      <c r="O33" s="33"/>
+      <c r="F33" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="G33" s="34"/>
+      <c r="H33" s="34"/>
+      <c r="I33" s="34"/>
+      <c r="J33" s="34"/>
+      <c r="K33" s="34"/>
+      <c r="L33" s="34"/>
+      <c r="M33" s="34"/>
+      <c r="N33" s="34"/>
+      <c r="O33" s="34"/>
     </row>
     <row r="34">
       <c r="A34" s="4"/>
@@ -34451,10 +34456,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
@@ -34478,8 +34483,8 @@
       <c r="A2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
       <c r="D2" s="8"/>
       <c r="E2" s="23"/>
       <c r="F2" s="4"/>
@@ -34495,10 +34500,10 @@
       <c r="A3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="34">
+      <c r="B3" s="35">
         <v>60.0</v>
       </c>
-      <c r="C3" s="34">
+      <c r="C3" s="35">
         <v>20.0</v>
       </c>
       <c r="D3" s="8">
@@ -34531,7 +34536,7 @@
     </row>
     <row r="5">
       <c r="A5" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
@@ -34573,7 +34578,7 @@
     </row>
     <row r="7">
       <c r="A7" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B7" s="8">
         <v>20.0</v>
@@ -34598,10 +34603,10 @@
     </row>
     <row r="8">
       <c r="A8" s="5"/>
-      <c r="B8" s="35"/>
-      <c r="C8" s="35"/>
-      <c r="D8" s="35"/>
-      <c r="E8" s="36"/>
+      <c r="B8" s="36"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="37"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
@@ -34632,10 +34637,10 @@
       <c r="A10" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="34">
+      <c r="B10" s="35">
         <v>4.0</v>
       </c>
-      <c r="C10" s="34">
+      <c r="C10" s="35">
         <v>15.0</v>
       </c>
       <c r="D10" s="8">
@@ -34657,10 +34662,10 @@
       <c r="A11" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="34">
+      <c r="B11" s="35">
         <v>18.0</v>
       </c>
-      <c r="C11" s="34">
+      <c r="C11" s="35">
         <v>15.0</v>
       </c>
       <c r="D11" s="8">
@@ -34712,13 +34717,13 @@
       <c r="A14" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="37" t="s">
-        <v>21</v>
+      <c r="B14" s="38" t="s">
+        <v>22</v>
       </c>
-      <c r="C14" s="37">
+      <c r="C14" s="38">
         <v>20.0</v>
       </c>
-      <c r="D14" s="37">
+      <c r="D14" s="38">
         <v>1.0</v>
       </c>
       <c r="E14" s="25">
@@ -34737,13 +34742,13 @@
       <c r="A15" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B15" s="37">
+      <c r="B15" s="38">
         <v>30.0</v>
       </c>
-      <c r="C15" s="37">
+      <c r="C15" s="38">
         <v>15.0</v>
       </c>
-      <c r="D15" s="37">
+      <c r="D15" s="38">
         <v>1.0</v>
       </c>
       <c r="E15" s="26"/>
@@ -34855,7 +34860,7 @@
         <v>46038.439073761576</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
@@ -34866,8 +34871,8 @@
       <c r="M20" s="4"/>
     </row>
     <row r="21">
-      <c r="A21" s="38" t="s">
-        <v>23</v>
+      <c r="A21" s="39" t="s">
+        <v>24</v>
       </c>
       <c r="B21" s="17"/>
       <c r="C21" s="17"/>
@@ -34884,15 +34889,15 @@
     </row>
     <row r="22">
       <c r="A22" s="7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
-      <c r="B22" s="34">
+      <c r="B22" s="35">
         <v>2.0</v>
       </c>
-      <c r="C22" s="34">
+      <c r="C22" s="35">
         <v>100.0</v>
       </c>
-      <c r="D22" s="34">
+      <c r="D22" s="35">
         <v>1.0</v>
       </c>
       <c r="E22" s="24">
@@ -34911,13 +34916,13 @@
       <c r="A23" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B23" s="34">
+      <c r="B23" s="35">
         <v>2.0</v>
       </c>
-      <c r="C23" s="34">
+      <c r="C23" s="35">
         <v>85.0</v>
       </c>
-      <c r="D23" s="34">
+      <c r="D23" s="35">
         <v>1.0</v>
       </c>
       <c r="E23" s="24">
@@ -34936,13 +34941,13 @@
       <c r="A24" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B24" s="34">
+      <c r="B24" s="35">
         <v>70.0</v>
       </c>
-      <c r="C24" s="34">
+      <c r="C24" s="35">
         <v>10.0</v>
       </c>
-      <c r="D24" s="34">
+      <c r="D24" s="35">
         <v>1.0</v>
       </c>
       <c r="E24" s="24">
@@ -34974,10 +34979,10 @@
     </row>
     <row r="26">
       <c r="A26" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
@@ -35015,13 +35020,13 @@
       <c r="M27" s="4"/>
     </row>
     <row r="28">
-      <c r="A28" s="39" t="s">
-        <v>27</v>
+      <c r="A28" s="40" t="s">
+        <v>28</v>
       </c>
-      <c r="B28" s="40"/>
-      <c r="C28" s="40"/>
-      <c r="D28" s="40"/>
-      <c r="E28" s="41"/>
+      <c r="B28" s="41"/>
+      <c r="C28" s="41"/>
+      <c r="D28" s="41"/>
+      <c r="E28" s="42"/>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
@@ -35032,10 +35037,10 @@
       <c r="M28" s="4"/>
     </row>
     <row r="29">
-      <c r="A29" s="42" t="s">
-        <v>28</v>
+      <c r="A29" s="33" t="s">
+        <v>29</v>
       </c>
-      <c r="B29" s="42">
+      <c r="B29" s="33">
         <v>100.0</v>
       </c>
       <c r="C29" s="15">
@@ -35057,8 +35062,8 @@
       <c r="M29" s="4"/>
     </row>
     <row r="30">
-      <c r="A30" s="33"/>
-      <c r="B30" s="33"/>
+      <c r="A30" s="34"/>
+      <c r="B30" s="34"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
@@ -35072,10 +35077,10 @@
       <c r="M30" s="4"/>
     </row>
     <row r="31">
-      <c r="A31" s="42" t="s">
-        <v>29</v>
+      <c r="A31" s="33" t="s">
+        <v>30</v>
       </c>
-      <c r="B31" s="33"/>
+      <c r="B31" s="34"/>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
@@ -35092,7 +35097,7 @@
       <c r="A32" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B32" s="42">
+      <c r="B32" s="33">
         <v>50.0</v>
       </c>
       <c r="C32" s="15">
@@ -35114,10 +35119,10 @@
       <c r="M32" s="4"/>
     </row>
     <row r="33">
-      <c r="A33" s="42" t="s">
-        <v>30</v>
+      <c r="A33" s="33" t="s">
+        <v>31</v>
       </c>
-      <c r="B33" s="42">
+      <c r="B33" s="33">
         <v>3.0</v>
       </c>
       <c r="C33" s="15">
@@ -35137,8 +35142,8 @@
       <c r="M33" s="4"/>
     </row>
     <row r="34">
-      <c r="A34" s="33"/>
-      <c r="B34" s="33"/>
+      <c r="A34" s="34"/>
+      <c r="B34" s="34"/>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
@@ -35152,8 +35157,8 @@
       <c r="M34" s="4"/>
     </row>
     <row r="35">
-      <c r="A35" s="33"/>
-      <c r="B35" s="33"/>
+      <c r="A35" s="34"/>
+      <c r="B35" s="34"/>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
@@ -35167,8 +35172,8 @@
       <c r="M35" s="4"/>
     </row>
     <row r="36">
-      <c r="A36" s="33"/>
-      <c r="B36" s="33"/>
+      <c r="A36" s="34"/>
+      <c r="B36" s="34"/>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
@@ -35182,8 +35187,8 @@
       <c r="M36" s="4"/>
     </row>
     <row r="37">
-      <c r="A37" s="33"/>
-      <c r="B37" s="33"/>
+      <c r="A37" s="34"/>
+      <c r="B37" s="34"/>
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
@@ -35197,8 +35202,8 @@
       <c r="M37" s="4"/>
     </row>
     <row r="38">
-      <c r="A38" s="33"/>
-      <c r="B38" s="33"/>
+      <c r="A38" s="34"/>
+      <c r="B38" s="34"/>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
@@ -35212,8 +35217,8 @@
       <c r="M38" s="4"/>
     </row>
     <row r="39">
-      <c r="A39" s="33"/>
-      <c r="B39" s="33"/>
+      <c r="A39" s="34"/>
+      <c r="B39" s="34"/>
       <c r="C39" s="4"/>
       <c r="D39" s="4"/>
       <c r="E39" s="4"/>
@@ -35227,8 +35232,8 @@
       <c r="M39" s="4"/>
     </row>
     <row r="40">
-      <c r="A40" s="33"/>
-      <c r="B40" s="33"/>
+      <c r="A40" s="34"/>
+      <c r="B40" s="34"/>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
@@ -35242,8 +35247,8 @@
       <c r="M40" s="4"/>
     </row>
     <row r="41">
-      <c r="A41" s="33"/>
-      <c r="B41" s="33"/>
+      <c r="A41" s="34"/>
+      <c r="B41" s="34"/>
       <c r="C41" s="4"/>
       <c r="D41" s="4"/>
       <c r="E41" s="4"/>
@@ -35257,8 +35262,8 @@
       <c r="M41" s="4"/>
     </row>
     <row r="42">
-      <c r="A42" s="33"/>
-      <c r="B42" s="33"/>
+      <c r="A42" s="34"/>
+      <c r="B42" s="34"/>
       <c r="C42" s="4"/>
       <c r="D42" s="4"/>
       <c r="E42" s="4"/>
@@ -35272,8 +35277,8 @@
       <c r="M42" s="4"/>
     </row>
     <row r="43">
-      <c r="A43" s="33"/>
-      <c r="B43" s="33"/>
+      <c r="A43" s="34"/>
+      <c r="B43" s="34"/>
       <c r="C43" s="4"/>
       <c r="D43" s="4"/>
       <c r="E43" s="4"/>
@@ -35287,8 +35292,8 @@
       <c r="M43" s="4"/>
     </row>
     <row r="44">
-      <c r="A44" s="33"/>
-      <c r="B44" s="33"/>
+      <c r="A44" s="34"/>
+      <c r="B44" s="34"/>
       <c r="C44" s="4"/>
       <c r="D44" s="4"/>
       <c r="E44" s="4"/>
@@ -35302,8 +35307,8 @@
       <c r="M44" s="4"/>
     </row>
     <row r="45">
-      <c r="A45" s="33"/>
-      <c r="B45" s="33"/>
+      <c r="A45" s="34"/>
+      <c r="B45" s="34"/>
       <c r="C45" s="4"/>
       <c r="D45" s="4"/>
       <c r="E45" s="4"/>
@@ -35317,8 +35322,8 @@
       <c r="M45" s="4"/>
     </row>
     <row r="46">
-      <c r="A46" s="33"/>
-      <c r="B46" s="33"/>
+      <c r="A46" s="34"/>
+      <c r="B46" s="34"/>
       <c r="C46" s="4"/>
       <c r="D46" s="4"/>
       <c r="E46" s="4"/>

</xml_diff>

<commit_message>
Update Laser.xlsx from Google Sheets @ 2026-01-21T05:25:33.666Z
</commit_message>
<xml_diff>
--- a/Laser.xlsx
+++ b/Laser.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="32">
   <si>
     <t>項目</t>
   </si>
@@ -760,16 +760,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="11">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="C7" s="11">
-        <v>10.0</v>
+        <v>5.0</v>
       </c>
       <c r="D7" s="11">
         <v>1.0</v>
       </c>
       <c r="E7" s="14">
-        <v>45957.92965825232</v>
+        <v>46042.0</v>
       </c>
       <c r="F7" s="15"/>
       <c r="G7" s="15"/>
@@ -783,19 +783,19 @@
     </row>
     <row r="8">
       <c r="A8" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="11">
-        <v>25.0</v>
+        <v>4.0</v>
       </c>
       <c r="C8" s="11">
-        <v>5.0</v>
+        <v>10.0</v>
       </c>
       <c r="D8" s="11">
         <v>1.0</v>
       </c>
       <c r="E8" s="14">
-        <v>45954.915123425926</v>
+        <v>45957.92965825232</v>
       </c>
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
@@ -808,13 +808,23 @@
       <c r="N8" s="4"/>
     </row>
     <row r="9">
-      <c r="A9" s="16"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
+      <c r="A9" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="11">
+        <v>25.0</v>
+      </c>
+      <c r="C9" s="11">
+        <v>5.0</v>
+      </c>
+      <c r="D9" s="11">
+        <v>1.0</v>
+      </c>
+      <c r="E9" s="14">
+        <v>45954.915123425926</v>
+      </c>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
@@ -824,12 +834,10 @@
       <c r="N9" s="4"/>
     </row>
     <row r="10">
-      <c r="A10" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="17"/>
+      <c r="A10" s="16"/>
+      <c r="B10" s="8"/>
       <c r="C10" s="17"/>
-      <c r="D10" s="8"/>
+      <c r="D10" s="17"/>
       <c r="E10" s="9"/>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
@@ -842,19 +850,13 @@
       <c r="N10" s="4"/>
     </row>
     <row r="11">
-      <c r="A11" s="7" t="s">
-        <v>6</v>
+      <c r="A11" s="5" t="s">
+        <v>10</v>
       </c>
-      <c r="B11" s="8">
-        <v>5.0</v>
-      </c>
-      <c r="C11" s="8">
-        <v>15.0</v>
-      </c>
-      <c r="D11" s="8">
-        <v>1.0</v>
-      </c>
-      <c r="E11" s="6"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="9"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
@@ -867,13 +869,13 @@
     </row>
     <row r="12">
       <c r="A12" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B12" s="8">
-        <v>32.0</v>
+        <v>5.0</v>
       </c>
       <c r="C12" s="8">
-        <v>5.0</v>
+        <v>15.0</v>
       </c>
       <c r="D12" s="8">
         <v>1.0</v>
@@ -890,10 +892,18 @@
       <c r="N12" s="4"/>
     </row>
     <row r="13">
-      <c r="A13" s="16"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
+      <c r="A13" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="8">
+        <v>32.0</v>
+      </c>
+      <c r="C13" s="8">
+        <v>5.0</v>
+      </c>
+      <c r="D13" s="8">
+        <v>1.0</v>
+      </c>
       <c r="E13" s="6"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
@@ -906,13 +916,11 @@
       <c r="N13" s="4"/>
     </row>
     <row r="14">
-      <c r="A14" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="12"/>
+      <c r="A14" s="16"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="6"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
@@ -924,18 +932,12 @@
       <c r="N14" s="4"/>
     </row>
     <row r="15">
-      <c r="A15" s="13" t="s">
-        <v>6</v>
+      <c r="A15" s="10" t="s">
+        <v>11</v>
       </c>
-      <c r="B15" s="11">
-        <v>5.0</v>
-      </c>
-      <c r="C15" s="11">
-        <v>5.0</v>
-      </c>
-      <c r="D15" s="11">
-        <v>1.0</v>
-      </c>
+      <c r="B15" s="18"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
       <c r="E15" s="12"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
@@ -949,10 +951,10 @@
     </row>
     <row r="16">
       <c r="A16" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B16" s="11">
-        <v>50.0</v>
+        <v>5.0</v>
       </c>
       <c r="C16" s="11">
         <v>5.0</v>
@@ -972,11 +974,19 @@
       <c r="N16" s="4"/>
     </row>
     <row r="17">
-      <c r="A17" s="16"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="6"/>
+      <c r="A17" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="11">
+        <v>50.0</v>
+      </c>
+      <c r="C17" s="11">
+        <v>5.0</v>
+      </c>
+      <c r="D17" s="11">
+        <v>1.0</v>
+      </c>
+      <c r="E17" s="12"/>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
@@ -988,9 +998,7 @@
       <c r="N17" s="4"/>
     </row>
     <row r="18">
-      <c r="A18" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="A18" s="16"/>
       <c r="B18" s="17"/>
       <c r="C18" s="17"/>
       <c r="D18" s="17"/>
@@ -1006,18 +1014,12 @@
       <c r="N18" s="4"/>
     </row>
     <row r="19">
-      <c r="A19" s="7" t="s">
-        <v>6</v>
+      <c r="A19" s="5" t="s">
+        <v>12</v>
       </c>
-      <c r="B19" s="8">
-        <v>5.0</v>
-      </c>
-      <c r="C19" s="8">
-        <v>5.0</v>
-      </c>
-      <c r="D19" s="8">
-        <v>1.0</v>
-      </c>
+      <c r="B19" s="17"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
       <c r="E19" s="6"/>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
@@ -1031,11 +1033,17 @@
     </row>
     <row r="20">
       <c r="A20" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
-      <c r="B20" s="17"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
+      <c r="B20" s="8">
+        <v>5.0</v>
+      </c>
+      <c r="C20" s="8">
+        <v>5.0</v>
+      </c>
+      <c r="D20" s="8">
+        <v>1.0</v>
+      </c>
       <c r="E20" s="6"/>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
@@ -1048,7 +1056,9 @@
       <c r="N20" s="4"/>
     </row>
     <row r="21">
-      <c r="A21" s="16"/>
+      <c r="A21" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="B21" s="17"/>
       <c r="C21" s="17"/>
       <c r="D21" s="17"/>
@@ -1064,13 +1074,11 @@
       <c r="N21" s="4"/>
     </row>
     <row r="22">
-      <c r="A22" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B22" s="18"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="12"/>
+      <c r="A22" s="16"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="6"/>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
@@ -1082,18 +1090,12 @@
       <c r="N22" s="4"/>
     </row>
     <row r="23">
-      <c r="A23" s="13" t="s">
-        <v>6</v>
+      <c r="A23" s="10" t="s">
+        <v>13</v>
       </c>
-      <c r="B23" s="11">
-        <v>5.0</v>
-      </c>
-      <c r="C23" s="11">
-        <v>5.0</v>
-      </c>
-      <c r="D23" s="11">
-        <v>1.0</v>
-      </c>
+      <c r="B23" s="18"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
       <c r="E23" s="12"/>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
@@ -1106,17 +1108,19 @@
       <c r="N23" s="4"/>
     </row>
     <row r="24">
-      <c r="A24" s="19" t="s">
-        <v>7</v>
+      <c r="A24" s="13" t="s">
+        <v>6</v>
       </c>
-      <c r="B24" s="20">
-        <v>55.0</v>
+      <c r="B24" s="11">
+        <v>5.0</v>
       </c>
-      <c r="C24" s="20">
-        <v>2.0</v>
+      <c r="C24" s="11">
+        <v>5.0</v>
       </c>
-      <c r="D24" s="21"/>
-      <c r="E24" s="22"/>
+      <c r="D24" s="11">
+        <v>1.0</v>
+      </c>
+      <c r="E24" s="12"/>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
@@ -1128,11 +1132,17 @@
       <c r="N24" s="4"/>
     </row>
     <row r="25">
-      <c r="A25" s="17"/>
-      <c r="B25" s="17"/>
-      <c r="C25" s="17"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="17"/>
+      <c r="A25" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" s="20">
+        <v>55.0</v>
+      </c>
+      <c r="C25" s="20">
+        <v>2.0</v>
+      </c>
+      <c r="D25" s="21"/>
+      <c r="E25" s="22"/>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
@@ -1224,11 +1234,11 @@
       <c r="N30" s="4"/>
     </row>
     <row r="31">
-      <c r="A31" s="4"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
+      <c r="A31" s="17"/>
+      <c r="B31" s="17"/>
+      <c r="C31" s="17"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="17"/>
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
       <c r="H31" s="4"/>
@@ -16982,6 +16992,22 @@
       <c r="L1015" s="4"/>
       <c r="M1015" s="4"/>
       <c r="N1015" s="4"/>
+    </row>
+    <row r="1016">
+      <c r="A1016" s="4"/>
+      <c r="B1016" s="4"/>
+      <c r="C1016" s="4"/>
+      <c r="D1016" s="4"/>
+      <c r="E1016" s="4"/>
+      <c r="F1016" s="4"/>
+      <c r="G1016" s="4"/>
+      <c r="H1016" s="4"/>
+      <c r="I1016" s="4"/>
+      <c r="J1016" s="4"/>
+      <c r="K1016" s="4"/>
+      <c r="L1016" s="4"/>
+      <c r="M1016" s="4"/>
+      <c r="N1016" s="4"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Update Laser.xlsx from Google Sheets @ 2026-01-21T05:25:56.698Z
</commit_message>
<xml_diff>
--- a/Laser.xlsx
+++ b/Laser.xlsx
@@ -868,18 +868,10 @@
       <c r="N11" s="4"/>
     </row>
     <row r="12">
-      <c r="A12" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="8">
-        <v>5.0</v>
-      </c>
-      <c r="C12" s="8">
-        <v>15.0</v>
-      </c>
-      <c r="D12" s="8">
-        <v>1.0</v>
-      </c>
+      <c r="A12" s="7"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
       <c r="E12" s="6"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
@@ -893,13 +885,13 @@
     </row>
     <row r="13">
       <c r="A13" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B13" s="8">
-        <v>32.0</v>
+        <v>5.0</v>
       </c>
       <c r="C13" s="8">
-        <v>5.0</v>
+        <v>15.0</v>
       </c>
       <c r="D13" s="8">
         <v>1.0</v>
@@ -916,10 +908,18 @@
       <c r="N13" s="4"/>
     </row>
     <row r="14">
-      <c r="A14" s="16"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
+      <c r="A14" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="8">
+        <v>32.0</v>
+      </c>
+      <c r="C14" s="8">
+        <v>5.0</v>
+      </c>
+      <c r="D14" s="8">
+        <v>1.0</v>
+      </c>
       <c r="E14" s="6"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
@@ -932,13 +932,11 @@
       <c r="N14" s="4"/>
     </row>
     <row r="15">
-      <c r="A15" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" s="18"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="12"/>
+      <c r="A15" s="16"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="6"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
@@ -950,18 +948,12 @@
       <c r="N15" s="4"/>
     </row>
     <row r="16">
-      <c r="A16" s="13" t="s">
-        <v>6</v>
+      <c r="A16" s="10" t="s">
+        <v>11</v>
       </c>
-      <c r="B16" s="11">
-        <v>5.0</v>
-      </c>
-      <c r="C16" s="11">
-        <v>5.0</v>
-      </c>
-      <c r="D16" s="11">
-        <v>1.0</v>
-      </c>
+      <c r="B16" s="18"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
       <c r="E16" s="12"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
@@ -975,10 +967,10 @@
     </row>
     <row r="17">
       <c r="A17" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B17" s="11">
-        <v>50.0</v>
+        <v>5.0</v>
       </c>
       <c r="C17" s="11">
         <v>5.0</v>
@@ -998,11 +990,19 @@
       <c r="N17" s="4"/>
     </row>
     <row r="18">
-      <c r="A18" s="16"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="6"/>
+      <c r="A18" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="11">
+        <v>50.0</v>
+      </c>
+      <c r="C18" s="11">
+        <v>5.0</v>
+      </c>
+      <c r="D18" s="11">
+        <v>1.0</v>
+      </c>
+      <c r="E18" s="12"/>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
@@ -1014,9 +1014,7 @@
       <c r="N18" s="4"/>
     </row>
     <row r="19">
-      <c r="A19" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="A19" s="16"/>
       <c r="B19" s="17"/>
       <c r="C19" s="17"/>
       <c r="D19" s="17"/>
@@ -1032,18 +1030,12 @@
       <c r="N19" s="4"/>
     </row>
     <row r="20">
-      <c r="A20" s="7" t="s">
-        <v>6</v>
+      <c r="A20" s="5" t="s">
+        <v>12</v>
       </c>
-      <c r="B20" s="8">
-        <v>5.0</v>
-      </c>
-      <c r="C20" s="8">
-        <v>5.0</v>
-      </c>
-      <c r="D20" s="8">
-        <v>1.0</v>
-      </c>
+      <c r="B20" s="17"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
       <c r="E20" s="6"/>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
@@ -1057,11 +1049,17 @@
     </row>
     <row r="21">
       <c r="A21" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
-      <c r="B21" s="17"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
+      <c r="B21" s="8">
+        <v>5.0</v>
+      </c>
+      <c r="C21" s="8">
+        <v>5.0</v>
+      </c>
+      <c r="D21" s="8">
+        <v>1.0</v>
+      </c>
       <c r="E21" s="6"/>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
@@ -1074,7 +1072,9 @@
       <c r="N21" s="4"/>
     </row>
     <row r="22">
-      <c r="A22" s="16"/>
+      <c r="A22" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="B22" s="17"/>
       <c r="C22" s="17"/>
       <c r="D22" s="17"/>
@@ -1090,13 +1090,11 @@
       <c r="N22" s="4"/>
     </row>
     <row r="23">
-      <c r="A23" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B23" s="18"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="12"/>
+      <c r="A23" s="16"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="6"/>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
@@ -1108,18 +1106,12 @@
       <c r="N23" s="4"/>
     </row>
     <row r="24">
-      <c r="A24" s="13" t="s">
-        <v>6</v>
+      <c r="A24" s="10" t="s">
+        <v>13</v>
       </c>
-      <c r="B24" s="11">
-        <v>5.0</v>
-      </c>
-      <c r="C24" s="11">
-        <v>5.0</v>
-      </c>
-      <c r="D24" s="11">
-        <v>1.0</v>
-      </c>
+      <c r="B24" s="18"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
       <c r="E24" s="12"/>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
@@ -1132,17 +1124,19 @@
       <c r="N24" s="4"/>
     </row>
     <row r="25">
-      <c r="A25" s="19" t="s">
-        <v>7</v>
+      <c r="A25" s="13" t="s">
+        <v>6</v>
       </c>
-      <c r="B25" s="20">
-        <v>55.0</v>
+      <c r="B25" s="11">
+        <v>5.0</v>
       </c>
-      <c r="C25" s="20">
-        <v>2.0</v>
+      <c r="C25" s="11">
+        <v>5.0</v>
       </c>
-      <c r="D25" s="21"/>
-      <c r="E25" s="22"/>
+      <c r="D25" s="11">
+        <v>1.0</v>
+      </c>
+      <c r="E25" s="12"/>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
@@ -1154,11 +1148,17 @@
       <c r="N25" s="4"/>
     </row>
     <row r="26">
-      <c r="A26" s="17"/>
-      <c r="B26" s="17"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="17"/>
+      <c r="A26" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" s="20">
+        <v>55.0</v>
+      </c>
+      <c r="C26" s="20">
+        <v>2.0</v>
+      </c>
+      <c r="D26" s="21"/>
+      <c r="E26" s="22"/>
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
@@ -1250,11 +1250,11 @@
       <c r="N31" s="4"/>
     </row>
     <row r="32">
-      <c r="A32" s="4"/>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
+      <c r="A32" s="17"/>
+      <c r="B32" s="17"/>
+      <c r="C32" s="17"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="17"/>
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
       <c r="H32" s="4"/>
@@ -17008,6 +17008,22 @@
       <c r="L1016" s="4"/>
       <c r="M1016" s="4"/>
       <c r="N1016" s="4"/>
+    </row>
+    <row r="1017">
+      <c r="A1017" s="4"/>
+      <c r="B1017" s="4"/>
+      <c r="C1017" s="4"/>
+      <c r="D1017" s="4"/>
+      <c r="E1017" s="4"/>
+      <c r="F1017" s="4"/>
+      <c r="G1017" s="4"/>
+      <c r="H1017" s="4"/>
+      <c r="I1017" s="4"/>
+      <c r="J1017" s="4"/>
+      <c r="K1017" s="4"/>
+      <c r="L1017" s="4"/>
+      <c r="M1017" s="4"/>
+      <c r="N1017" s="4"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Update Laser.xlsx from Google Sheets @ 2026-01-21T05:26:00.594Z
</commit_message>
<xml_diff>
--- a/Laser.xlsx
+++ b/Laser.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="32">
   <si>
     <t>項目</t>
   </si>
@@ -868,13 +868,23 @@
       <c r="N11" s="4"/>
     </row>
     <row r="12">
-      <c r="A12" s="7"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
+      <c r="A12" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="11">
+        <v>5.0</v>
+      </c>
+      <c r="C12" s="11">
+        <v>5.0</v>
+      </c>
+      <c r="D12" s="11">
+        <v>1.0</v>
+      </c>
+      <c r="E12" s="14">
+        <v>46042.0</v>
+      </c>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>

</xml_diff>

<commit_message>
Update Laser.xlsx from Google Sheets @ 2026-01-21T05:26:04.724Z
</commit_message>
<xml_diff>
--- a/Laser.xlsx
+++ b/Laser.xlsx
@@ -868,19 +868,19 @@
       <c r="N11" s="4"/>
     </row>
     <row r="12">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="11">
+      <c r="B12" s="8">
         <v>5.0</v>
       </c>
-      <c r="C12" s="11">
+      <c r="C12" s="8">
         <v>5.0</v>
       </c>
-      <c r="D12" s="11">
+      <c r="D12" s="8">
         <v>1.0</v>
       </c>
-      <c r="E12" s="14">
+      <c r="E12" s="9">
         <v>46042.0</v>
       </c>
       <c r="F12" s="15"/>

</xml_diff>

<commit_message>
Update Laser.xlsx from Google Sheets @ 2026-01-21T05:26:09.908Z
</commit_message>
<xml_diff>
--- a/Laser.xlsx
+++ b/Laser.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="32">
   <si>
     <t>項目</t>
   </si>
@@ -760,16 +760,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="11">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
       <c r="C7" s="11">
-        <v>5.0</v>
+        <v>10.0</v>
       </c>
       <c r="D7" s="11">
         <v>1.0</v>
       </c>
       <c r="E7" s="14">
-        <v>46042.0</v>
+        <v>45957.92965825232</v>
       </c>
       <c r="F7" s="15"/>
       <c r="G7" s="15"/>
@@ -783,19 +783,19 @@
     </row>
     <row r="8">
       <c r="A8" s="13" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" s="11">
-        <v>4.0</v>
+        <v>25.0</v>
       </c>
       <c r="C8" s="11">
-        <v>10.0</v>
+        <v>5.0</v>
       </c>
       <c r="D8" s="11">
         <v>1.0</v>
       </c>
       <c r="E8" s="14">
-        <v>45957.92965825232</v>
+        <v>45954.915123425926</v>
       </c>
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
@@ -808,23 +808,13 @@
       <c r="N8" s="4"/>
     </row>
     <row r="9">
-      <c r="A9" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="11">
-        <v>25.0</v>
-      </c>
-      <c r="C9" s="11">
-        <v>5.0</v>
-      </c>
-      <c r="D9" s="11">
-        <v>1.0</v>
-      </c>
-      <c r="E9" s="14">
-        <v>45954.915123425926</v>
-      </c>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
+      <c r="A9" s="16"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
@@ -834,10 +824,12 @@
       <c r="N9" s="4"/>
     </row>
     <row r="10">
-      <c r="A10" s="16"/>
-      <c r="B10" s="8"/>
+      <c r="A10" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="17"/>
       <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
+      <c r="D10" s="8"/>
       <c r="E10" s="9"/>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
@@ -850,15 +842,23 @@
       <c r="N10" s="4"/>
     </row>
     <row r="11">
-      <c r="A11" s="5" t="s">
-        <v>10</v>
+      <c r="A11" s="7" t="s">
+        <v>6</v>
       </c>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
+      <c r="B11" s="8">
+        <v>5.0</v>
+      </c>
+      <c r="C11" s="8">
+        <v>5.0</v>
+      </c>
+      <c r="D11" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="E11" s="9">
+        <v>46042.0</v>
+      </c>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
@@ -875,16 +875,14 @@
         <v>5.0</v>
       </c>
       <c r="C12" s="8">
-        <v>5.0</v>
+        <v>15.0</v>
       </c>
       <c r="D12" s="8">
         <v>1.0</v>
       </c>
-      <c r="E12" s="9">
-        <v>46042.0</v>
-      </c>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
@@ -895,13 +893,13 @@
     </row>
     <row r="13">
       <c r="A13" s="7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B13" s="8">
-        <v>5.0</v>
+        <v>32.0</v>
       </c>
       <c r="C13" s="8">
-        <v>15.0</v>
+        <v>5.0</v>
       </c>
       <c r="D13" s="8">
         <v>1.0</v>
@@ -918,18 +916,10 @@
       <c r="N13" s="4"/>
     </row>
     <row r="14">
-      <c r="A14" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="8">
-        <v>32.0</v>
-      </c>
-      <c r="C14" s="8">
-        <v>5.0</v>
-      </c>
-      <c r="D14" s="8">
-        <v>1.0</v>
-      </c>
+      <c r="A14" s="16"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
       <c r="E14" s="6"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
@@ -942,11 +932,13 @@
       <c r="N14" s="4"/>
     </row>
     <row r="15">
-      <c r="A15" s="16"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="6"/>
+      <c r="A15" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="18"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="12"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
@@ -958,12 +950,18 @@
       <c r="N15" s="4"/>
     </row>
     <row r="16">
-      <c r="A16" s="10" t="s">
-        <v>11</v>
+      <c r="A16" s="13" t="s">
+        <v>6</v>
       </c>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
+      <c r="B16" s="11">
+        <v>5.0</v>
+      </c>
+      <c r="C16" s="11">
+        <v>5.0</v>
+      </c>
+      <c r="D16" s="11">
+        <v>1.0</v>
+      </c>
       <c r="E16" s="12"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
@@ -977,10 +975,10 @@
     </row>
     <row r="17">
       <c r="A17" s="13" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B17" s="11">
-        <v>5.0</v>
+        <v>50.0</v>
       </c>
       <c r="C17" s="11">
         <v>5.0</v>
@@ -1000,19 +998,11 @@
       <c r="N17" s="4"/>
     </row>
     <row r="18">
-      <c r="A18" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B18" s="11">
-        <v>50.0</v>
-      </c>
-      <c r="C18" s="11">
-        <v>5.0</v>
-      </c>
-      <c r="D18" s="11">
-        <v>1.0</v>
-      </c>
-      <c r="E18" s="12"/>
+      <c r="A18" s="16"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="6"/>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
@@ -1024,7 +1014,9 @@
       <c r="N18" s="4"/>
     </row>
     <row r="19">
-      <c r="A19" s="16"/>
+      <c r="A19" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="B19" s="17"/>
       <c r="C19" s="17"/>
       <c r="D19" s="17"/>
@@ -1040,12 +1032,18 @@
       <c r="N19" s="4"/>
     </row>
     <row r="20">
-      <c r="A20" s="5" t="s">
-        <v>12</v>
+      <c r="A20" s="7" t="s">
+        <v>6</v>
       </c>
-      <c r="B20" s="17"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
+      <c r="B20" s="8">
+        <v>5.0</v>
+      </c>
+      <c r="C20" s="8">
+        <v>5.0</v>
+      </c>
+      <c r="D20" s="8">
+        <v>1.0</v>
+      </c>
       <c r="E20" s="6"/>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
@@ -1059,17 +1057,11 @@
     </row>
     <row r="21">
       <c r="A21" s="7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
-      <c r="B21" s="8">
-        <v>5.0</v>
-      </c>
-      <c r="C21" s="8">
-        <v>5.0</v>
-      </c>
-      <c r="D21" s="8">
-        <v>1.0</v>
-      </c>
+      <c r="B21" s="17"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
       <c r="E21" s="6"/>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
@@ -1082,9 +1074,7 @@
       <c r="N21" s="4"/>
     </row>
     <row r="22">
-      <c r="A22" s="7" t="s">
-        <v>7</v>
-      </c>
+      <c r="A22" s="16"/>
       <c r="B22" s="17"/>
       <c r="C22" s="17"/>
       <c r="D22" s="17"/>
@@ -1100,11 +1090,13 @@
       <c r="N22" s="4"/>
     </row>
     <row r="23">
-      <c r="A23" s="16"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="6"/>
+      <c r="A23" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="18"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="12"/>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
@@ -1116,12 +1108,18 @@
       <c r="N23" s="4"/>
     </row>
     <row r="24">
-      <c r="A24" s="10" t="s">
-        <v>13</v>
+      <c r="A24" s="13" t="s">
+        <v>6</v>
       </c>
-      <c r="B24" s="18"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
+      <c r="B24" s="11">
+        <v>5.0</v>
+      </c>
+      <c r="C24" s="11">
+        <v>5.0</v>
+      </c>
+      <c r="D24" s="11">
+        <v>1.0</v>
+      </c>
       <c r="E24" s="12"/>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
@@ -1134,19 +1132,17 @@
       <c r="N24" s="4"/>
     </row>
     <row r="25">
-      <c r="A25" s="13" t="s">
-        <v>6</v>
+      <c r="A25" s="19" t="s">
+        <v>7</v>
       </c>
-      <c r="B25" s="11">
-        <v>5.0</v>
+      <c r="B25" s="20">
+        <v>55.0</v>
       </c>
-      <c r="C25" s="11">
-        <v>5.0</v>
+      <c r="C25" s="20">
+        <v>2.0</v>
       </c>
-      <c r="D25" s="11">
-        <v>1.0</v>
-      </c>
-      <c r="E25" s="12"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="22"/>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
@@ -1158,17 +1154,11 @@
       <c r="N25" s="4"/>
     </row>
     <row r="26">
-      <c r="A26" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="B26" s="20">
-        <v>55.0</v>
-      </c>
-      <c r="C26" s="20">
-        <v>2.0</v>
-      </c>
-      <c r="D26" s="21"/>
-      <c r="E26" s="22"/>
+      <c r="A26" s="17"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
@@ -1260,11 +1250,11 @@
       <c r="N31" s="4"/>
     </row>
     <row r="32">
-      <c r="A32" s="17"/>
-      <c r="B32" s="17"/>
-      <c r="C32" s="17"/>
-      <c r="D32" s="17"/>
-      <c r="E32" s="17"/>
+      <c r="A32" s="4"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
       <c r="H32" s="4"/>
@@ -17018,22 +17008,6 @@
       <c r="L1016" s="4"/>
       <c r="M1016" s="4"/>
       <c r="N1016" s="4"/>
-    </row>
-    <row r="1017">
-      <c r="A1017" s="4"/>
-      <c r="B1017" s="4"/>
-      <c r="C1017" s="4"/>
-      <c r="D1017" s="4"/>
-      <c r="E1017" s="4"/>
-      <c r="F1017" s="4"/>
-      <c r="G1017" s="4"/>
-      <c r="H1017" s="4"/>
-      <c r="I1017" s="4"/>
-      <c r="J1017" s="4"/>
-      <c r="K1017" s="4"/>
-      <c r="L1017" s="4"/>
-      <c r="M1017" s="4"/>
-      <c r="N1017" s="4"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Update Laser.xlsx from Google Sheets @ 2026-01-21T16:16:43.498Z
</commit_message>
<xml_diff>
--- a/Laser.xlsx
+++ b/Laser.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="33">
   <si>
     <t>項目</t>
   </si>
@@ -109,6 +109,9 @@
   </si>
   <si>
     <t>紙</t>
+  </si>
+  <si>
+    <t>生日牌</t>
   </si>
 </sst>
 </file>
@@ -35184,7 +35187,9 @@
       <c r="M34" s="4"/>
     </row>
     <row r="35">
-      <c r="A35" s="34"/>
+      <c r="A35" s="33" t="s">
+        <v>32</v>
+      </c>
       <c r="B35" s="34"/>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>

</xml_diff>

<commit_message>
Update Laser.xlsx from Google Sheets @ 2026-01-21T16:16:49.894Z
</commit_message>
<xml_diff>
--- a/Laser.xlsx
+++ b/Laser.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="33">
   <si>
     <t>項目</t>
   </si>
@@ -35190,10 +35190,14 @@
       <c r="A35" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="B35" s="34"/>
+      <c r="B35" s="33" t="s">
+        <v>12</v>
+      </c>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
+      <c r="E35" s="43">
+        <v>46044.0116671875</v>
+      </c>
       <c r="F35" s="4"/>
       <c r="G35" s="4"/>
       <c r="H35" s="4"/>

</xml_diff>

<commit_message>
Update Laser.xlsx from Google Sheets @ 2026-01-21T16:17:59.928Z
</commit_message>
<xml_diff>
--- a/Laser.xlsx
+++ b/Laser.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="34">
   <si>
     <t>項目</t>
   </si>
@@ -112,6 +112,9 @@
   </si>
   <si>
     <t>生日牌</t>
+  </si>
+  <si>
+    <t>雕刻</t>
   </si>
 </sst>
 </file>
@@ -35208,7 +35211,9 @@
       <c r="M35" s="4"/>
     </row>
     <row r="36">
-      <c r="A36" s="34"/>
+      <c r="A36" s="33" t="s">
+        <v>33</v>
+      </c>
       <c r="B36" s="34"/>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>

</xml_diff>

<commit_message>
Update Laser.xlsx from Google Sheets @ 2026-01-21T16:18:03.714Z
</commit_message>
<xml_diff>
--- a/Laser.xlsx
+++ b/Laser.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="35">
   <si>
     <t>項目</t>
   </si>
@@ -115,6 +115,9 @@
   </si>
   <si>
     <t>雕刻</t>
+  </si>
+  <si>
+    <t>刻線</t>
   </si>
 </sst>
 </file>
@@ -35228,7 +35231,9 @@
       <c r="M36" s="4"/>
     </row>
     <row r="37">
-      <c r="A37" s="34"/>
+      <c r="A37" s="33" t="s">
+        <v>34</v>
+      </c>
       <c r="B37" s="34"/>
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>

</xml_diff>

<commit_message>
Update Laser.xlsx from Google Sheets @ 2026-01-21T16:18:11.373Z
</commit_message>
<xml_diff>
--- a/Laser.xlsx
+++ b/Laser.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="35">
   <si>
     <t>項目</t>
   </si>
@@ -35248,7 +35248,9 @@
       <c r="M37" s="4"/>
     </row>
     <row r="38">
-      <c r="A38" s="34"/>
+      <c r="A38" s="33" t="s">
+        <v>21</v>
+      </c>
       <c r="B38" s="34"/>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>

</xml_diff>

<commit_message>
Update Laser.xlsx from Google Sheets @ 2026-01-21T16:18:47.882Z
</commit_message>
<xml_diff>
--- a/Laser.xlsx
+++ b/Laser.xlsx
@@ -35217,7 +35217,9 @@
       <c r="A36" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="B36" s="34"/>
+      <c r="B36" s="33">
+        <v>5.0</v>
+      </c>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>

</xml_diff>

<commit_message>
Update Laser.xlsx from Google Sheets @ 2026-01-21T16:18:53.946Z
</commit_message>
<xml_diff>
--- a/Laser.xlsx
+++ b/Laser.xlsx
@@ -35220,9 +35220,15 @@
       <c r="B36" s="33">
         <v>5.0</v>
       </c>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
+      <c r="C36" s="15">
+        <v>80.0</v>
+      </c>
+      <c r="D36" s="15">
+        <v>1.0</v>
+      </c>
+      <c r="E36" s="43">
+        <v>46044.01310700232</v>
+      </c>
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>
       <c r="H36" s="4"/>

</xml_diff>

<commit_message>
Update Laser.xlsx from Google Sheets @ 2026-01-21T16:18:57.653Z
</commit_message>
<xml_diff>
--- a/Laser.xlsx
+++ b/Laser.xlsx
@@ -35242,8 +35242,12 @@
       <c r="A37" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="B37" s="34"/>
-      <c r="C37" s="4"/>
+      <c r="B37" s="33">
+        <v>15.0</v>
+      </c>
+      <c r="C37" s="15">
+        <v>10.0</v>
+      </c>
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>

</xml_diff>

<commit_message>
Update Laser.xlsx from Google Sheets @ 2026-01-21T16:18:59.904Z
</commit_message>
<xml_diff>
--- a/Laser.xlsx
+++ b/Laser.xlsx
@@ -35248,8 +35248,12 @@
       <c r="C37" s="15">
         <v>10.0</v>
       </c>
-      <c r="D37" s="4"/>
-      <c r="E37" s="4"/>
+      <c r="D37" s="15">
+        <v>1.0</v>
+      </c>
+      <c r="E37" s="43">
+        <v>46044.01316956019</v>
+      </c>
       <c r="F37" s="4"/>
       <c r="G37" s="4"/>
       <c r="H37" s="4"/>

</xml_diff>

<commit_message>
Update Laser.xlsx from Google Sheets @ 2026-01-21T16:19:04.969Z
</commit_message>
<xml_diff>
--- a/Laser.xlsx
+++ b/Laser.xlsx
@@ -35252,7 +35252,7 @@
         <v>1.0</v>
       </c>
       <c r="E37" s="43">
-        <v>46044.01316956019</v>
+        <v>46044.013194907406</v>
       </c>
       <c r="F37" s="4"/>
       <c r="G37" s="4"/>
@@ -35267,7 +35267,9 @@
       <c r="A38" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="B38" s="34"/>
+      <c r="B38" s="33">
+        <v>20.0</v>
+      </c>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>

</xml_diff>

<commit_message>
Update Laser.xlsx from Google Sheets @ 2026-01-21T16:19:07.495Z
</commit_message>
<xml_diff>
--- a/Laser.xlsx
+++ b/Laser.xlsx
@@ -35270,9 +35270,15 @@
       <c r="B38" s="33">
         <v>20.0</v>
       </c>
-      <c r="C38" s="4"/>
-      <c r="D38" s="4"/>
-      <c r="E38" s="4"/>
+      <c r="C38" s="15">
+        <v>10.0</v>
+      </c>
+      <c r="D38" s="15">
+        <v>4.0</v>
+      </c>
+      <c r="E38" s="43">
+        <v>46044.01323650463</v>
+      </c>
       <c r="F38" s="4"/>
       <c r="G38" s="4"/>
       <c r="H38" s="4"/>

</xml_diff>

<commit_message>
Update Laser.xlsx from Google Sheets @ 2026-01-21T16:19:30.036Z
</commit_message>
<xml_diff>
--- a/Laser.xlsx
+++ b/Laser.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="35">
   <si>
     <t>項目</t>
   </si>
@@ -35304,8 +35304,12 @@
       <c r="M39" s="4"/>
     </row>
     <row r="40">
-      <c r="A40" s="34"/>
-      <c r="B40" s="34"/>
+      <c r="A40" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B40" s="33" t="s">
+        <v>12</v>
+      </c>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
@@ -35319,10 +35323,18 @@
       <c r="M40" s="4"/>
     </row>
     <row r="41">
-      <c r="A41" s="34"/>
-      <c r="B41" s="34"/>
-      <c r="C41" s="4"/>
-      <c r="D41" s="4"/>
+      <c r="A41" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="B41" s="33">
+        <v>5.0</v>
+      </c>
+      <c r="C41" s="15">
+        <v>80.0</v>
+      </c>
+      <c r="D41" s="15">
+        <v>1.0</v>
+      </c>
       <c r="E41" s="4"/>
       <c r="F41" s="4"/>
       <c r="G41" s="4"/>
@@ -35334,10 +35346,18 @@
       <c r="M41" s="4"/>
     </row>
     <row r="42">
-      <c r="A42" s="34"/>
-      <c r="B42" s="34"/>
-      <c r="C42" s="4"/>
-      <c r="D42" s="4"/>
+      <c r="A42" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="B42" s="33">
+        <v>15.0</v>
+      </c>
+      <c r="C42" s="15">
+        <v>10.0</v>
+      </c>
+      <c r="D42" s="15">
+        <v>1.0</v>
+      </c>
       <c r="E42" s="4"/>
       <c r="F42" s="4"/>
       <c r="G42" s="4"/>
@@ -35349,10 +35369,18 @@
       <c r="M42" s="4"/>
     </row>
     <row r="43">
-      <c r="A43" s="34"/>
-      <c r="B43" s="34"/>
-      <c r="C43" s="4"/>
-      <c r="D43" s="4"/>
+      <c r="A43" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="B43" s="33">
+        <v>20.0</v>
+      </c>
+      <c r="C43" s="15">
+        <v>10.0</v>
+      </c>
+      <c r="D43" s="15">
+        <v>4.0</v>
+      </c>
       <c r="E43" s="4"/>
       <c r="F43" s="4"/>
       <c r="G43" s="4"/>

</xml_diff>

<commit_message>
Update Laser.xlsx from Google Sheets @ 2026-01-21T16:19:39.824Z
</commit_message>
<xml_diff>
--- a/Laser.xlsx
+++ b/Laser.xlsx
@@ -35308,11 +35308,13 @@
         <v>32</v>
       </c>
       <c r="B40" s="33" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
-      <c r="E40" s="4"/>
+      <c r="E40" s="43">
+        <v>46044.0136399537</v>
+      </c>
       <c r="F40" s="4"/>
       <c r="G40" s="4"/>
       <c r="H40" s="4"/>

</xml_diff>

<commit_message>
Update Laser.xlsx from Google Sheets @ 2026-01-21T16:19:51.911Z
</commit_message>
<xml_diff>
--- a/Laser.xlsx
+++ b/Laser.xlsx
@@ -35381,9 +35381,11 @@
         <v>10.0</v>
       </c>
       <c r="D43" s="15">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
-      <c r="E43" s="4"/>
+      <c r="E43" s="43">
+        <v>46044.01378171296</v>
+      </c>
       <c r="F43" s="4"/>
       <c r="G43" s="4"/>
       <c r="H43" s="4"/>

</xml_diff>

<commit_message>
Update Laser.xlsx from Google Sheets @ 2026-01-21T16:20:12.295Z
</commit_message>
<xml_diff>
--- a/Laser.xlsx
+++ b/Laser.xlsx
@@ -35381,10 +35381,10 @@
         <v>10.0</v>
       </c>
       <c r="D43" s="15">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
       <c r="E43" s="43">
-        <v>46044.01378171296</v>
+        <v>46044.014003055556</v>
       </c>
       <c r="F43" s="4"/>
       <c r="G43" s="4"/>

</xml_diff>

<commit_message>
Update Laser.xlsx from Google Sheets @ 2026-01-29T15:04:18.194Z
</commit_message>
<xml_diff>
--- a/Laser.xlsx
+++ b/Laser.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="36">
   <si>
     <t>項目</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>4mm</t>
+  </si>
+  <si>
+    <t>A4紙</t>
   </si>
   <si>
     <t>(PS)</t>
@@ -1179,7 +1182,9 @@
       <c r="N26" s="4"/>
     </row>
     <row r="27">
-      <c r="A27" s="17"/>
+      <c r="A27" s="8" t="s">
+        <v>14</v>
+      </c>
       <c r="B27" s="17"/>
       <c r="C27" s="17"/>
       <c r="D27" s="17"/>
@@ -1195,7 +1200,9 @@
       <c r="N27" s="4"/>
     </row>
     <row r="28">
-      <c r="A28" s="17"/>
+      <c r="A28" s="8" t="s">
+        <v>6</v>
+      </c>
       <c r="B28" s="17"/>
       <c r="C28" s="17"/>
       <c r="D28" s="17"/>
@@ -17134,7 +17141,7 @@
     </row>
     <row r="5">
       <c r="A5" s="7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
@@ -17293,7 +17300,7 @@
     </row>
     <row r="12">
       <c r="A12" s="13" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B12" s="11">
         <v>4.0</v>
@@ -17320,7 +17327,7 @@
     </row>
     <row r="13">
       <c r="A13" s="13" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
@@ -17406,7 +17413,7 @@
         <v>10</v>
       </c>
       <c r="B17" s="28" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
@@ -17751,7 +17758,7 @@
     </row>
     <row r="33" ht="20.25" customHeight="1">
       <c r="A33" s="30" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B33" s="31">
         <v>5.0</v>
@@ -17766,7 +17773,7 @@
         <v>46043.55545597222</v>
       </c>
       <c r="F33" s="33" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G33" s="34"/>
       <c r="H33" s="34"/>
@@ -34492,10 +34499,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
@@ -34572,7 +34579,7 @@
     </row>
     <row r="5">
       <c r="A5" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
@@ -34614,7 +34621,7 @@
     </row>
     <row r="7">
       <c r="A7" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B7" s="8">
         <v>20.0</v>
@@ -34754,7 +34761,7 @@
         <v>6</v>
       </c>
       <c r="B14" s="38" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C14" s="38">
         <v>20.0</v>
@@ -34896,7 +34903,7 @@
         <v>46038.439073761576</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
@@ -34908,7 +34915,7 @@
     </row>
     <row r="21">
       <c r="A21" s="39" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B21" s="17"/>
       <c r="C21" s="17"/>
@@ -34925,7 +34932,7 @@
     </row>
     <row r="22">
       <c r="A22" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B22" s="35">
         <v>2.0</v>
@@ -35015,10 +35022,10 @@
     </row>
     <row r="26">
       <c r="A26" s="7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
@@ -35057,7 +35064,7 @@
     </row>
     <row r="28">
       <c r="A28" s="40" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B28" s="41"/>
       <c r="C28" s="41"/>
@@ -35074,7 +35081,7 @@
     </row>
     <row r="29">
       <c r="A29" s="33" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B29" s="33">
         <v>100.0</v>
@@ -35114,7 +35121,7 @@
     </row>
     <row r="31">
       <c r="A31" s="33" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B31" s="34"/>
       <c r="C31" s="4"/>
@@ -35156,7 +35163,7 @@
     </row>
     <row r="33">
       <c r="A33" s="33" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B33" s="33">
         <v>3.0</v>
@@ -35194,7 +35201,7 @@
     </row>
     <row r="35">
       <c r="A35" s="33" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B35" s="33" t="s">
         <v>12</v>
@@ -35215,7 +35222,7 @@
     </row>
     <row r="36">
       <c r="A36" s="33" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B36" s="33">
         <v>5.0</v>
@@ -35240,7 +35247,7 @@
     </row>
     <row r="37">
       <c r="A37" s="33" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B37" s="33">
         <v>15.0</v>
@@ -35265,7 +35272,7 @@
     </row>
     <row r="38">
       <c r="A38" s="33" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B38" s="33">
         <v>20.0</v>
@@ -35305,10 +35312,10 @@
     </row>
     <row r="40">
       <c r="A40" s="33" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B40" s="33" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
@@ -35326,7 +35333,7 @@
     </row>
     <row r="41">
       <c r="A41" s="33" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B41" s="33">
         <v>5.0</v>
@@ -35349,7 +35356,7 @@
     </row>
     <row r="42">
       <c r="A42" s="33" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B42" s="33">
         <v>15.0</v>
@@ -35372,7 +35379,7 @@
     </row>
     <row r="43">
       <c r="A43" s="33" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B43" s="33">
         <v>20.0</v>

</xml_diff>

<commit_message>
Update Laser.xlsx from Google Sheets @ 2026-01-29T15:04:33.893Z
</commit_message>
<xml_diff>
--- a/Laser.xlsx
+++ b/Laser.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="37">
   <si>
     <t>項目</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>A4紙</t>
+  </si>
+  <si>
+    <t>(0.90 Power)</t>
   </si>
   <si>
     <t>(PS)</t>
@@ -280,7 +283,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -349,6 +352,9 @@
     </xf>
     <xf borderId="8" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="14" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
@@ -1185,10 +1191,14 @@
       <c r="A27" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B27" s="17"/>
+      <c r="B27" s="8" t="s">
+        <v>15</v>
+      </c>
       <c r="C27" s="17"/>
       <c r="D27" s="17"/>
-      <c r="E27" s="17"/>
+      <c r="E27" s="23">
+        <v>46051.96147880787</v>
+      </c>
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
@@ -17075,7 +17085,7 @@
       <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="23"/>
+      <c r="E2" s="24"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
@@ -17100,7 +17110,7 @@
       <c r="D3" s="8">
         <v>1.0</v>
       </c>
-      <c r="E3" s="24">
+      <c r="E3" s="25">
         <v>46037.00168581019</v>
       </c>
       <c r="F3" s="4"/>
@@ -17127,7 +17137,7 @@
       <c r="D4" s="8">
         <v>1.0</v>
       </c>
-      <c r="E4" s="23"/>
+      <c r="E4" s="24"/>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
@@ -17141,12 +17151,12 @@
     </row>
     <row r="5">
       <c r="A5" s="7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
-      <c r="E5" s="23"/>
+      <c r="E5" s="24"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
@@ -17171,7 +17181,7 @@
       <c r="D6" s="8">
         <v>1.0</v>
       </c>
-      <c r="E6" s="23"/>
+      <c r="E6" s="24"/>
       <c r="F6" s="15"/>
       <c r="G6" s="15"/>
       <c r="H6" s="15"/>
@@ -17196,7 +17206,7 @@
       <c r="D7" s="8">
         <v>1.0</v>
       </c>
-      <c r="E7" s="24"/>
+      <c r="E7" s="25"/>
       <c r="F7" s="15"/>
       <c r="G7" s="15"/>
       <c r="H7" s="15"/>
@@ -17213,7 +17223,7 @@
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
-      <c r="E8" s="24"/>
+      <c r="E8" s="25"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
@@ -17232,7 +17242,7 @@
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
-      <c r="E9" s="25"/>
+      <c r="E9" s="26"/>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
@@ -17257,7 +17267,7 @@
       <c r="D10" s="11">
         <v>1.0</v>
       </c>
-      <c r="E10" s="25">
+      <c r="E10" s="26">
         <v>45900.4876925</v>
       </c>
       <c r="F10" s="4"/>
@@ -17284,7 +17294,7 @@
       <c r="D11" s="11">
         <v>1.0</v>
       </c>
-      <c r="E11" s="25">
+      <c r="E11" s="26">
         <v>46031.84505053241</v>
       </c>
       <c r="F11" s="4"/>
@@ -17300,7 +17310,7 @@
     </row>
     <row r="12">
       <c r="A12" s="13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B12" s="11">
         <v>4.0</v>
@@ -17311,7 +17321,7 @@
       <c r="D12" s="11">
         <v>1.0</v>
       </c>
-      <c r="E12" s="25">
+      <c r="E12" s="26">
         <v>45960.0</v>
       </c>
       <c r="F12" s="4"/>
@@ -17327,12 +17337,12 @@
     </row>
     <row r="13">
       <c r="A13" s="13" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
       <c r="D13" s="11"/>
-      <c r="E13" s="26"/>
+      <c r="E13" s="27"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
@@ -17357,7 +17367,7 @@
       <c r="D14" s="11">
         <v>1.0</v>
       </c>
-      <c r="E14" s="26"/>
+      <c r="E14" s="27"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
@@ -17382,7 +17392,7 @@
       <c r="D15" s="11">
         <v>1.0</v>
       </c>
-      <c r="E15" s="26"/>
+      <c r="E15" s="27"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
@@ -17395,8 +17405,8 @@
       <c r="O15" s="4"/>
     </row>
     <row r="16">
-      <c r="A16" s="27"/>
-      <c r="E16" s="23"/>
+      <c r="A16" s="28"/>
+      <c r="E16" s="24"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
@@ -17412,12 +17422,12 @@
       <c r="A17" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="28" t="s">
-        <v>15</v>
+      <c r="B17" s="29" t="s">
+        <v>16</v>
       </c>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
-      <c r="E17" s="23"/>
+      <c r="E17" s="24"/>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
@@ -17442,7 +17452,7 @@
       <c r="D18" s="8">
         <v>1.0</v>
       </c>
-      <c r="E18" s="23"/>
+      <c r="E18" s="24"/>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
@@ -17467,7 +17477,7 @@
       <c r="D19" s="8">
         <v>1.0</v>
       </c>
-      <c r="E19" s="23"/>
+      <c r="E19" s="24"/>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
@@ -17484,7 +17494,7 @@
       <c r="B20" s="17"/>
       <c r="C20" s="17"/>
       <c r="D20" s="17"/>
-      <c r="E20" s="23"/>
+      <c r="E20" s="24"/>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
@@ -17503,7 +17513,7 @@
       <c r="B21" s="18"/>
       <c r="C21" s="18"/>
       <c r="D21" s="18"/>
-      <c r="E21" s="26"/>
+      <c r="E21" s="27"/>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
@@ -17528,7 +17538,7 @@
       <c r="D22" s="11">
         <v>1.0</v>
       </c>
-      <c r="E22" s="26"/>
+      <c r="E22" s="27"/>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
@@ -17553,7 +17563,7 @@
       <c r="D23" s="11">
         <v>2.0</v>
       </c>
-      <c r="E23" s="26"/>
+      <c r="E23" s="27"/>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
@@ -17570,7 +17580,7 @@
       <c r="B24" s="17"/>
       <c r="C24" s="17"/>
       <c r="D24" s="17"/>
-      <c r="E24" s="23"/>
+      <c r="E24" s="24"/>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
@@ -17589,7 +17599,7 @@
       <c r="B25" s="17"/>
       <c r="C25" s="17"/>
       <c r="D25" s="17"/>
-      <c r="E25" s="23"/>
+      <c r="E25" s="24"/>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
@@ -17614,7 +17624,7 @@
       <c r="D26" s="8">
         <v>1.0</v>
       </c>
-      <c r="E26" s="23"/>
+      <c r="E26" s="24"/>
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
@@ -17639,7 +17649,7 @@
       <c r="D27" s="8">
         <v>2.0</v>
       </c>
-      <c r="E27" s="24">
+      <c r="E27" s="25">
         <v>45974.8842990625</v>
       </c>
       <c r="F27" s="4"/>
@@ -17658,7 +17668,7 @@
       <c r="B28" s="17"/>
       <c r="C28" s="17"/>
       <c r="D28" s="17"/>
-      <c r="E28" s="23"/>
+      <c r="E28" s="24"/>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
@@ -17677,7 +17687,7 @@
       <c r="B29" s="18"/>
       <c r="C29" s="18"/>
       <c r="D29" s="18"/>
-      <c r="E29" s="26"/>
+      <c r="E29" s="27"/>
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
@@ -17702,7 +17712,7 @@
       <c r="D30" s="11">
         <v>1.0</v>
       </c>
-      <c r="E30" s="26"/>
+      <c r="E30" s="27"/>
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
@@ -17727,7 +17737,7 @@
       <c r="D31" s="20">
         <v>1.0</v>
       </c>
-      <c r="E31" s="29"/>
+      <c r="E31" s="30"/>
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
       <c r="H31" s="4"/>
@@ -17757,33 +17767,33 @@
       <c r="O32" s="4"/>
     </row>
     <row r="33" ht="20.25" customHeight="1">
-      <c r="A33" s="30" t="s">
-        <v>17</v>
+      <c r="A33" s="31" t="s">
+        <v>18</v>
       </c>
-      <c r="B33" s="31">
+      <c r="B33" s="32">
         <v>5.0</v>
       </c>
-      <c r="C33" s="31">
+      <c r="C33" s="32">
         <v>10.0</v>
       </c>
-      <c r="D33" s="31">
+      <c r="D33" s="32">
         <v>2.0</v>
       </c>
-      <c r="E33" s="32">
+      <c r="E33" s="33">
         <v>46043.55545597222</v>
       </c>
-      <c r="F33" s="33" t="s">
-        <v>18</v>
+      <c r="F33" s="34" t="s">
+        <v>19</v>
       </c>
-      <c r="G33" s="34"/>
-      <c r="H33" s="34"/>
-      <c r="I33" s="34"/>
-      <c r="J33" s="34"/>
-      <c r="K33" s="34"/>
-      <c r="L33" s="34"/>
-      <c r="M33" s="34"/>
-      <c r="N33" s="34"/>
-      <c r="O33" s="34"/>
+      <c r="G33" s="35"/>
+      <c r="H33" s="35"/>
+      <c r="I33" s="35"/>
+      <c r="J33" s="35"/>
+      <c r="K33" s="35"/>
+      <c r="L33" s="35"/>
+      <c r="M33" s="35"/>
+      <c r="N33" s="35"/>
+      <c r="O33" s="35"/>
     </row>
     <row r="34">
       <c r="A34" s="4"/>
@@ -34499,10 +34509,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
@@ -34526,10 +34536,10 @@
       <c r="A2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
       <c r="D2" s="8"/>
-      <c r="E2" s="23"/>
+      <c r="E2" s="24"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
@@ -34543,16 +34553,16 @@
       <c r="A3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="35">
+      <c r="B3" s="36">
         <v>60.0</v>
       </c>
-      <c r="C3" s="35">
+      <c r="C3" s="36">
         <v>20.0</v>
       </c>
       <c r="D3" s="8">
         <v>1.0</v>
       </c>
-      <c r="E3" s="23"/>
+      <c r="E3" s="24"/>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
@@ -34567,7 +34577,7 @@
       <c r="B4" s="17"/>
       <c r="C4" s="17"/>
       <c r="D4" s="17"/>
-      <c r="E4" s="23"/>
+      <c r="E4" s="24"/>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
@@ -34579,12 +34589,12 @@
     </row>
     <row r="5">
       <c r="A5" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
-      <c r="E5" s="23"/>
+      <c r="E5" s="24"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
@@ -34607,7 +34617,7 @@
       <c r="D6" s="8">
         <v>1.0</v>
       </c>
-      <c r="E6" s="24">
+      <c r="E6" s="25">
         <v>45946.87939769676</v>
       </c>
       <c r="F6" s="4"/>
@@ -34621,7 +34631,7 @@
     </row>
     <row r="7">
       <c r="A7" s="7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B7" s="8">
         <v>20.0</v>
@@ -34632,7 +34642,7 @@
       <c r="D7" s="8">
         <v>1.0</v>
       </c>
-      <c r="E7" s="24">
+      <c r="E7" s="25">
         <v>45946.879225324075</v>
       </c>
       <c r="F7" s="4"/>
@@ -34646,10 +34656,10 @@
     </row>
     <row r="8">
       <c r="A8" s="5"/>
-      <c r="B8" s="36"/>
-      <c r="C8" s="36"/>
-      <c r="D8" s="36"/>
-      <c r="E8" s="37"/>
+      <c r="B8" s="37"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="38"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
@@ -34666,7 +34676,7 @@
       <c r="B9" s="17"/>
       <c r="C9" s="17"/>
       <c r="D9" s="17"/>
-      <c r="E9" s="23"/>
+      <c r="E9" s="24"/>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
@@ -34680,16 +34690,16 @@
       <c r="A10" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="35">
+      <c r="B10" s="36">
         <v>4.0</v>
       </c>
-      <c r="C10" s="35">
+      <c r="C10" s="36">
         <v>15.0</v>
       </c>
       <c r="D10" s="8">
         <v>1.0</v>
       </c>
-      <c r="E10" s="24">
+      <c r="E10" s="25">
         <v>46009.0</v>
       </c>
       <c r="F10" s="4"/>
@@ -34705,16 +34715,16 @@
       <c r="A11" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="35">
+      <c r="B11" s="36">
         <v>18.0</v>
       </c>
-      <c r="C11" s="35">
+      <c r="C11" s="36">
         <v>15.0</v>
       </c>
       <c r="D11" s="8">
         <v>1.0</v>
       </c>
-      <c r="E11" s="23"/>
+      <c r="E11" s="24"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
@@ -34729,7 +34739,7 @@
       <c r="B12" s="17"/>
       <c r="C12" s="17"/>
       <c r="D12" s="17"/>
-      <c r="E12" s="23"/>
+      <c r="E12" s="24"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
@@ -34746,7 +34756,7 @@
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
       <c r="D13" s="11"/>
-      <c r="E13" s="26"/>
+      <c r="E13" s="27"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
@@ -34760,16 +34770,16 @@
       <c r="A14" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="38" t="s">
-        <v>23</v>
+      <c r="B14" s="39" t="s">
+        <v>24</v>
       </c>
-      <c r="C14" s="38">
+      <c r="C14" s="39">
         <v>20.0</v>
       </c>
-      <c r="D14" s="38">
+      <c r="D14" s="39">
         <v>1.0</v>
       </c>
-      <c r="E14" s="25">
+      <c r="E14" s="26">
         <v>46006.93993954861</v>
       </c>
       <c r="F14" s="4"/>
@@ -34785,16 +34795,16 @@
       <c r="A15" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B15" s="38">
+      <c r="B15" s="39">
         <v>30.0</v>
       </c>
-      <c r="C15" s="38">
+      <c r="C15" s="39">
         <v>15.0</v>
       </c>
-      <c r="D15" s="38">
+      <c r="D15" s="39">
         <v>1.0</v>
       </c>
-      <c r="E15" s="26"/>
+      <c r="E15" s="27"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
@@ -34809,7 +34819,7 @@
       <c r="B16" s="17"/>
       <c r="C16" s="17"/>
       <c r="D16" s="17"/>
-      <c r="E16" s="23"/>
+      <c r="E16" s="24"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
@@ -34826,7 +34836,7 @@
       <c r="B17" s="17"/>
       <c r="C17" s="17"/>
       <c r="D17" s="17"/>
-      <c r="E17" s="23"/>
+      <c r="E17" s="24"/>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
@@ -34849,7 +34859,7 @@
       <c r="D18" s="8">
         <v>1.0</v>
       </c>
-      <c r="E18" s="24">
+      <c r="E18" s="25">
         <v>46006.95620635417</v>
       </c>
       <c r="F18" s="4"/>
@@ -34874,7 +34884,7 @@
       <c r="D19" s="8">
         <v>1.0</v>
       </c>
-      <c r="E19" s="24">
+      <c r="E19" s="25">
         <v>46006.95627618056</v>
       </c>
       <c r="F19" s="4"/>
@@ -34899,11 +34909,11 @@
       <c r="D20" s="8">
         <v>1.0</v>
       </c>
-      <c r="E20" s="24">
+      <c r="E20" s="25">
         <v>46038.439073761576</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
@@ -34914,13 +34924,13 @@
       <c r="M20" s="4"/>
     </row>
     <row r="21">
-      <c r="A21" s="39" t="s">
-        <v>25</v>
+      <c r="A21" s="40" t="s">
+        <v>26</v>
       </c>
       <c r="B21" s="17"/>
       <c r="C21" s="17"/>
       <c r="D21" s="17"/>
-      <c r="E21" s="23"/>
+      <c r="E21" s="24"/>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
@@ -34932,18 +34942,18 @@
     </row>
     <row r="22">
       <c r="A22" s="7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
-      <c r="B22" s="35">
+      <c r="B22" s="36">
         <v>2.0</v>
       </c>
-      <c r="C22" s="35">
+      <c r="C22" s="36">
         <v>100.0</v>
       </c>
-      <c r="D22" s="35">
+      <c r="D22" s="36">
         <v>1.0</v>
       </c>
-      <c r="E22" s="24">
+      <c r="E22" s="25">
         <v>45900.48749</v>
       </c>
       <c r="F22" s="4"/>
@@ -34959,16 +34969,16 @@
       <c r="A23" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B23" s="35">
+      <c r="B23" s="36">
         <v>2.0</v>
       </c>
-      <c r="C23" s="35">
+      <c r="C23" s="36">
         <v>85.0</v>
       </c>
-      <c r="D23" s="35">
+      <c r="D23" s="36">
         <v>1.0</v>
       </c>
-      <c r="E23" s="24">
+      <c r="E23" s="25">
         <v>45900.48745738426</v>
       </c>
       <c r="F23" s="4"/>
@@ -34984,16 +34994,16 @@
       <c r="A24" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B24" s="35">
+      <c r="B24" s="36">
         <v>70.0</v>
       </c>
-      <c r="C24" s="35">
+      <c r="C24" s="36">
         <v>10.0</v>
       </c>
-      <c r="D24" s="35">
+      <c r="D24" s="36">
         <v>1.0</v>
       </c>
-      <c r="E24" s="24">
+      <c r="E24" s="25">
         <v>45900.48752491898</v>
       </c>
       <c r="F24" s="4"/>
@@ -35010,7 +35020,7 @@
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
-      <c r="E25" s="23"/>
+      <c r="E25" s="24"/>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
@@ -35022,14 +35032,14 @@
     </row>
     <row r="26">
       <c r="A26" s="7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
-      <c r="E26" s="24">
+      <c r="E26" s="25">
         <v>45946.87875708334</v>
       </c>
       <c r="F26" s="4"/>
@@ -35050,7 +35060,7 @@
       </c>
       <c r="C27" s="17"/>
       <c r="D27" s="17"/>
-      <c r="E27" s="24">
+      <c r="E27" s="25">
         <v>45946.87887299768</v>
       </c>
       <c r="F27" s="4"/>
@@ -35063,13 +35073,13 @@
       <c r="M27" s="4"/>
     </row>
     <row r="28">
-      <c r="A28" s="40" t="s">
-        <v>29</v>
+      <c r="A28" s="41" t="s">
+        <v>30</v>
       </c>
-      <c r="B28" s="41"/>
-      <c r="C28" s="41"/>
-      <c r="D28" s="41"/>
-      <c r="E28" s="42"/>
+      <c r="B28" s="42"/>
+      <c r="C28" s="42"/>
+      <c r="D28" s="42"/>
+      <c r="E28" s="43"/>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
@@ -35080,10 +35090,10 @@
       <c r="M28" s="4"/>
     </row>
     <row r="29">
-      <c r="A29" s="33" t="s">
-        <v>30</v>
+      <c r="A29" s="34" t="s">
+        <v>31</v>
       </c>
-      <c r="B29" s="33">
+      <c r="B29" s="34">
         <v>100.0</v>
       </c>
       <c r="C29" s="15">
@@ -35092,7 +35102,7 @@
       <c r="D29" s="15">
         <v>2.0</v>
       </c>
-      <c r="E29" s="43">
+      <c r="E29" s="44">
         <v>46009.783484375</v>
       </c>
       <c r="F29" s="4"/>
@@ -35105,8 +35115,8 @@
       <c r="M29" s="4"/>
     </row>
     <row r="30">
-      <c r="A30" s="34"/>
-      <c r="B30" s="34"/>
+      <c r="A30" s="35"/>
+      <c r="B30" s="35"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
@@ -35120,10 +35130,10 @@
       <c r="M30" s="4"/>
     </row>
     <row r="31">
-      <c r="A31" s="33" t="s">
-        <v>31</v>
+      <c r="A31" s="34" t="s">
+        <v>32</v>
       </c>
-      <c r="B31" s="34"/>
+      <c r="B31" s="35"/>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
@@ -35140,7 +35150,7 @@
       <c r="A32" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B32" s="33">
+      <c r="B32" s="34">
         <v>50.0</v>
       </c>
       <c r="C32" s="15">
@@ -35149,7 +35159,7 @@
       <c r="D32" s="15">
         <v>1.0</v>
       </c>
-      <c r="E32" s="43">
+      <c r="E32" s="44">
         <v>46038.9559609375</v>
       </c>
       <c r="F32" s="4"/>
@@ -35162,17 +35172,17 @@
       <c r="M32" s="4"/>
     </row>
     <row r="33">
-      <c r="A33" s="33" t="s">
-        <v>32</v>
+      <c r="A33" s="34" t="s">
+        <v>33</v>
       </c>
-      <c r="B33" s="33">
+      <c r="B33" s="34">
         <v>3.0</v>
       </c>
       <c r="C33" s="15">
         <v>80.0</v>
       </c>
       <c r="D33" s="4"/>
-      <c r="E33" s="43">
+      <c r="E33" s="44">
         <v>46042.92027434028</v>
       </c>
       <c r="F33" s="4"/>
@@ -35185,8 +35195,8 @@
       <c r="M33" s="4"/>
     </row>
     <row r="34">
-      <c r="A34" s="34"/>
-      <c r="B34" s="34"/>
+      <c r="A34" s="35"/>
+      <c r="B34" s="35"/>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
@@ -35200,15 +35210,15 @@
       <c r="M34" s="4"/>
     </row>
     <row r="35">
-      <c r="A35" s="33" t="s">
-        <v>33</v>
+      <c r="A35" s="34" t="s">
+        <v>34</v>
       </c>
-      <c r="B35" s="33" t="s">
+      <c r="B35" s="34" t="s">
         <v>12</v>
       </c>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
-      <c r="E35" s="43">
+      <c r="E35" s="44">
         <v>46044.0116671875</v>
       </c>
       <c r="F35" s="4"/>
@@ -35221,10 +35231,10 @@
       <c r="M35" s="4"/>
     </row>
     <row r="36">
-      <c r="A36" s="33" t="s">
-        <v>34</v>
+      <c r="A36" s="34" t="s">
+        <v>35</v>
       </c>
-      <c r="B36" s="33">
+      <c r="B36" s="34">
         <v>5.0</v>
       </c>
       <c r="C36" s="15">
@@ -35233,7 +35243,7 @@
       <c r="D36" s="15">
         <v>1.0</v>
       </c>
-      <c r="E36" s="43">
+      <c r="E36" s="44">
         <v>46044.01310700232</v>
       </c>
       <c r="F36" s="4"/>
@@ -35246,10 +35256,10 @@
       <c r="M36" s="4"/>
     </row>
     <row r="37">
-      <c r="A37" s="33" t="s">
-        <v>35</v>
+      <c r="A37" s="34" t="s">
+        <v>36</v>
       </c>
-      <c r="B37" s="33">
+      <c r="B37" s="34">
         <v>15.0</v>
       </c>
       <c r="C37" s="15">
@@ -35258,7 +35268,7 @@
       <c r="D37" s="15">
         <v>1.0</v>
       </c>
-      <c r="E37" s="43">
+      <c r="E37" s="44">
         <v>46044.013194907406</v>
       </c>
       <c r="F37" s="4"/>
@@ -35271,10 +35281,10 @@
       <c r="M37" s="4"/>
     </row>
     <row r="38">
-      <c r="A38" s="33" t="s">
-        <v>22</v>
+      <c r="A38" s="34" t="s">
+        <v>23</v>
       </c>
-      <c r="B38" s="33">
+      <c r="B38" s="34">
         <v>20.0</v>
       </c>
       <c r="C38" s="15">
@@ -35283,7 +35293,7 @@
       <c r="D38" s="15">
         <v>4.0</v>
       </c>
-      <c r="E38" s="43">
+      <c r="E38" s="44">
         <v>46044.01393202547</v>
       </c>
       <c r="F38" s="4"/>
@@ -35296,8 +35306,8 @@
       <c r="M38" s="4"/>
     </row>
     <row r="39">
-      <c r="A39" s="34"/>
-      <c r="B39" s="34"/>
+      <c r="A39" s="35"/>
+      <c r="B39" s="35"/>
       <c r="C39" s="4"/>
       <c r="D39" s="4"/>
       <c r="E39" s="4"/>
@@ -35311,15 +35321,15 @@
       <c r="M39" s="4"/>
     </row>
     <row r="40">
-      <c r="A40" s="33" t="s">
-        <v>33</v>
+      <c r="A40" s="34" t="s">
+        <v>34</v>
       </c>
-      <c r="B40" s="33" t="s">
-        <v>25</v>
+      <c r="B40" s="34" t="s">
+        <v>26</v>
       </c>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
-      <c r="E40" s="43">
+      <c r="E40" s="44">
         <v>46044.0136399537</v>
       </c>
       <c r="F40" s="4"/>
@@ -35332,10 +35342,10 @@
       <c r="M40" s="4"/>
     </row>
     <row r="41">
-      <c r="A41" s="33" t="s">
-        <v>34</v>
+      <c r="A41" s="34" t="s">
+        <v>35</v>
       </c>
-      <c r="B41" s="33">
+      <c r="B41" s="34">
         <v>5.0</v>
       </c>
       <c r="C41" s="15">
@@ -35355,10 +35365,10 @@
       <c r="M41" s="4"/>
     </row>
     <row r="42">
-      <c r="A42" s="33" t="s">
-        <v>35</v>
+      <c r="A42" s="34" t="s">
+        <v>36</v>
       </c>
-      <c r="B42" s="33">
+      <c r="B42" s="34">
         <v>15.0</v>
       </c>
       <c r="C42" s="15">
@@ -35378,10 +35388,10 @@
       <c r="M42" s="4"/>
     </row>
     <row r="43">
-      <c r="A43" s="33" t="s">
-        <v>22</v>
+      <c r="A43" s="34" t="s">
+        <v>23</v>
       </c>
-      <c r="B43" s="33">
+      <c r="B43" s="34">
         <v>20.0</v>
       </c>
       <c r="C43" s="15">
@@ -35390,7 +35400,7 @@
       <c r="D43" s="15">
         <v>6.0</v>
       </c>
-      <c r="E43" s="43">
+      <c r="E43" s="44">
         <v>46044.014003055556</v>
       </c>
       <c r="F43" s="4"/>
@@ -35403,8 +35413,8 @@
       <c r="M43" s="4"/>
     </row>
     <row r="44">
-      <c r="A44" s="34"/>
-      <c r="B44" s="34"/>
+      <c r="A44" s="35"/>
+      <c r="B44" s="35"/>
       <c r="C44" s="4"/>
       <c r="D44" s="4"/>
       <c r="E44" s="4"/>
@@ -35418,8 +35428,8 @@
       <c r="M44" s="4"/>
     </row>
     <row r="45">
-      <c r="A45" s="34"/>
-      <c r="B45" s="34"/>
+      <c r="A45" s="35"/>
+      <c r="B45" s="35"/>
       <c r="C45" s="4"/>
       <c r="D45" s="4"/>
       <c r="E45" s="4"/>
@@ -35433,8 +35443,8 @@
       <c r="M45" s="4"/>
     </row>
     <row r="46">
-      <c r="A46" s="34"/>
-      <c r="B46" s="34"/>
+      <c r="A46" s="35"/>
+      <c r="B46" s="35"/>
       <c r="C46" s="4"/>
       <c r="D46" s="4"/>
       <c r="E46" s="4"/>

</xml_diff>

<commit_message>
Update Laser.xlsx from Google Sheets @ 2026-01-29T15:04:40.668Z
</commit_message>
<xml_diff>
--- a/Laser.xlsx
+++ b/Laser.xlsx
@@ -60,7 +60,7 @@
     <t>A4紙</t>
   </si>
   <si>
-    <t>(0.90 Power)</t>
+    <t>(0.9 Power)</t>
   </si>
   <si>
     <t>(PS)</t>
@@ -1197,7 +1197,7 @@
       <c r="C27" s="17"/>
       <c r="D27" s="17"/>
       <c r="E27" s="23">
-        <v>46051.96147880787</v>
+        <v>46051.96156388889</v>
       </c>
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>

</xml_diff>

<commit_message>
Update Laser.xlsx from Google Sheets @ 2026-01-29T15:04:49.059Z
</commit_message>
<xml_diff>
--- a/Laser.xlsx
+++ b/Laser.xlsx
@@ -1213,10 +1213,14 @@
       <c r="A28" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B28" s="17"/>
+      <c r="B28" s="8">
+        <v>3.0</v>
+      </c>
       <c r="C28" s="17"/>
       <c r="D28" s="17"/>
-      <c r="E28" s="17"/>
+      <c r="E28" s="23">
+        <v>46051.961634293984</v>
+      </c>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>

</xml_diff>

<commit_message>
Update Laser.xlsx from Google Sheets @ 2026-01-29T15:05:01.816Z
</commit_message>
<xml_diff>
--- a/Laser.xlsx
+++ b/Laser.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="37">
   <si>
     <t>項目</t>
   </si>
@@ -63,6 +63,9 @@
     <t>(0.9 Power)</t>
   </si>
   <si>
+    <t>Cut</t>
+  </si>
+  <si>
     <t>(PS)</t>
   </si>
   <si>
@@ -82,9 +85,6 @@
   </si>
   <si>
     <t>0.3 mm</t>
-  </si>
-  <si>
-    <t>Cut</t>
   </si>
   <si>
     <t>６</t>
@@ -1214,12 +1214,14 @@
         <v>6</v>
       </c>
       <c r="B28" s="8">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
-      <c r="C28" s="17"/>
+      <c r="C28" s="8">
+        <v>300.0</v>
+      </c>
       <c r="D28" s="17"/>
       <c r="E28" s="23">
-        <v>46051.961634293984</v>
+        <v>46051.96181112269</v>
       </c>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
@@ -1232,7 +1234,9 @@
       <c r="N28" s="4"/>
     </row>
     <row r="29">
-      <c r="A29" s="17"/>
+      <c r="A29" s="8" t="s">
+        <v>16</v>
+      </c>
       <c r="B29" s="17"/>
       <c r="C29" s="17"/>
       <c r="D29" s="17"/>
@@ -17155,7 +17159,7 @@
     </row>
     <row r="5">
       <c r="A5" s="7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
@@ -17314,7 +17318,7 @@
     </row>
     <row r="12">
       <c r="A12" s="13" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B12" s="11">
         <v>4.0</v>
@@ -17341,7 +17345,7 @@
     </row>
     <row r="13">
       <c r="A13" s="13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
@@ -17427,7 +17431,7 @@
         <v>10</v>
       </c>
       <c r="B17" s="29" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
@@ -17772,7 +17776,7 @@
     </row>
     <row r="33" ht="20.25" customHeight="1">
       <c r="A33" s="31" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B33" s="32">
         <v>5.0</v>
@@ -17787,7 +17791,7 @@
         <v>46043.55545597222</v>
       </c>
       <c r="F33" s="34" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G33" s="35"/>
       <c r="H33" s="35"/>
@@ -34513,10 +34517,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
@@ -34593,7 +34597,7 @@
     </row>
     <row r="5">
       <c r="A5" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
@@ -34635,7 +34639,7 @@
     </row>
     <row r="7">
       <c r="A7" s="7" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B7" s="8">
         <v>20.0</v>
@@ -35286,7 +35290,7 @@
     </row>
     <row r="38">
       <c r="A38" s="34" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B38" s="34">
         <v>20.0</v>
@@ -35393,7 +35397,7 @@
     </row>
     <row r="43">
       <c r="A43" s="34" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B43" s="34">
         <v>20.0</v>

</xml_diff>

<commit_message>
Update Laser.xlsx from Google Sheets @ 2026-01-29T15:05:05.306Z
</commit_message>
<xml_diff>
--- a/Laser.xlsx
+++ b/Laser.xlsx
@@ -1237,8 +1237,12 @@
       <c r="A29" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B29" s="17"/>
-      <c r="C29" s="17"/>
+      <c r="B29" s="8">
+        <v>20.0</v>
+      </c>
+      <c r="C29" s="8">
+        <v>300.0</v>
+      </c>
       <c r="D29" s="17"/>
       <c r="E29" s="17"/>
       <c r="F29" s="4"/>

</xml_diff>

<commit_message>
Update Laser.xlsx from Google Sheets @ 2026-01-29T15:05:10.982Z
</commit_message>
<xml_diff>
--- a/Laser.xlsx
+++ b/Laser.xlsx
@@ -1244,7 +1244,9 @@
         <v>300.0</v>
       </c>
       <c r="D29" s="17"/>
-      <c r="E29" s="17"/>
+      <c r="E29" s="23">
+        <v>46051.96188216435</v>
+      </c>
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>

</xml_diff>

<commit_message>
Update Laser.xlsx from Google Sheets @ 2026-02-03T08:37:48.755Z
</commit_message>
<xml_diff>
--- a/Laser.xlsx
+++ b/Laser.xlsx
@@ -35299,7 +35299,7 @@
         <v>16</v>
       </c>
       <c r="B38" s="34">
-        <v>20.0</v>
+        <v>25.0</v>
       </c>
       <c r="C38" s="15">
         <v>10.0</v>
@@ -35308,7 +35308,7 @@
         <v>4.0</v>
       </c>
       <c r="E38" s="44">
-        <v>46044.01393202547</v>
+        <v>46056.69291506945</v>
       </c>
       <c r="F38" s="4"/>
       <c r="G38" s="4"/>

</xml_diff>

<commit_message>
Update Laser.xlsx from Google Sheets @ 2026-02-03T08:37:56.372Z
</commit_message>
<xml_diff>
--- a/Laser.xlsx
+++ b/Laser.xlsx
@@ -35305,10 +35305,10 @@
         <v>10.0</v>
       </c>
       <c r="D38" s="15">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
       <c r="E38" s="44">
-        <v>46056.69291506945</v>
+        <v>46056.69299506945</v>
       </c>
       <c r="F38" s="4"/>
       <c r="G38" s="4"/>

</xml_diff>

<commit_message>
Update Laser.xlsx from Google Sheets @ 2026-02-03T08:50:52.313Z
</commit_message>
<xml_diff>
--- a/Laser.xlsx
+++ b/Laser.xlsx
@@ -35299,7 +35299,7 @@
         <v>16</v>
       </c>
       <c r="B38" s="34">
-        <v>25.0</v>
+        <v>30.0</v>
       </c>
       <c r="C38" s="15">
         <v>10.0</v>
@@ -35308,7 +35308,7 @@
         <v>1.0</v>
       </c>
       <c r="E38" s="44">
-        <v>46056.69299506945</v>
+        <v>46056.701985011576</v>
       </c>
       <c r="F38" s="4"/>
       <c r="G38" s="4"/>

</xml_diff>